<commit_message>
categories down to C
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E06DD-3011-4520-A342-79FF73981A38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930C8CDD-1A83-4FB6-985C-22368B1DF8E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11630" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB - Primary List" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ABB - Primary List'!$A$1:$T$413</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ABB - Supplementary Lists'!$A$1:$T$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Quick Tables'!$G$1:$H$5</definedName>
-    <definedName name="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R181" hidden="1">'ABB - Primary List'!$B$261:$N$261</definedName>
+    <definedName name="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R18" hidden="1">'ABB - Primary List'!$B$261:$N$261</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -241,7 +241,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range 1" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R181"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R18"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -6748,39 +6748,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787458D5-0D53-4EB5-974E-BD980B126E90}">
   <dimension ref="A1:T434"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.1796875" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1208</v>
       </c>
@@ -6901,7 +6901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1389</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1398</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1394</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1411</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1424</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1171</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>717</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>710</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>708</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1933</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1887</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>367</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>213</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>223</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>980</v>
       </c>
@@ -7774,7 +7774,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>47</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>861</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>253</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>37</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>36</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>34</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>688</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>406</v>
       </c>
@@ -8236,7 +8236,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>404</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>400</v>
       </c>
@@ -8354,7 +8354,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>10</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1215</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1210</v>
       </c>
@@ -8534,7 +8534,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1214</v>
       </c>
@@ -8593,7 +8593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1826</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>273</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1935</v>
       </c>
@@ -8773,7 +8773,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>864</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>228</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>702</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>645</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>647</v>
       </c>
@@ -9056,7 +9056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>640</v>
       </c>
@@ -9115,7 +9115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>583</v>
       </c>
@@ -9164,7 +9164,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>587</v>
       </c>
@@ -9213,7 +9213,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>582</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>584</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>337</v>
       </c>
@@ -9390,7 +9390,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1617</v>
       </c>
@@ -9449,7 +9449,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1614</v>
       </c>
@@ -9508,7 +9508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1625</v>
       </c>
@@ -9567,7 +9567,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1622</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1612</v>
       </c>
@@ -9673,7 +9673,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1613</v>
       </c>
@@ -9732,7 +9732,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>699</v>
       </c>
@@ -9791,7 +9791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>28</v>
       </c>
@@ -9850,7 +9850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>42</v>
       </c>
@@ -9909,7 +9909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>614</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>636</v>
       </c>
@@ -10030,7 +10030,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>274</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>629</v>
       </c>
@@ -10148,7 +10148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>853</v>
       </c>
@@ -10207,7 +10207,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>849</v>
       </c>
@@ -10266,7 +10266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>845</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>184</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>189</v>
       </c>
@@ -10446,7 +10446,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>186</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>346</v>
       </c>
@@ -10564,7 +10564,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>351</v>
       </c>
@@ -10623,7 +10623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>340</v>
       </c>
@@ -10682,7 +10682,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>344</v>
       </c>
@@ -10741,7 +10741,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>348</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>359</v>
       </c>
@@ -10859,7 +10859,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>343</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>350</v>
       </c>
@@ -10977,7 +10977,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>349</v>
       </c>
@@ -11036,7 +11036,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>358</v>
       </c>
@@ -11095,7 +11095,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>339</v>
       </c>
@@ -11154,7 +11154,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1250</v>
       </c>
@@ -11213,7 +11213,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>589</v>
       </c>
@@ -11262,7 +11262,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="2"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>819</v>
       </c>
@@ -11309,7 +11309,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>829</v>
       </c>
@@ -11368,7 +11368,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>825</v>
       </c>
@@ -11427,7 +11427,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1850</v>
       </c>
@@ -11474,7 +11474,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1696</v>
       </c>
@@ -11533,7 +11533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>161</v>
       </c>
@@ -11592,7 +11592,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>773</v>
       </c>
@@ -11651,7 +11651,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>134</v>
       </c>
@@ -11710,7 +11710,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>298</v>
       </c>
@@ -11769,7 +11769,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>303</v>
       </c>
@@ -11828,7 +11828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>300</v>
       </c>
@@ -11887,7 +11887,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>297</v>
       </c>
@@ -11946,7 +11946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>306</v>
       </c>
@@ -11995,7 +11995,7 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="2"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>43</v>
       </c>
@@ -12054,7 +12054,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1890</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>444</v>
       </c>
@@ -12160,7 +12160,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>446</v>
       </c>
@@ -12219,7 +12219,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>411</v>
       </c>
@@ -12278,7 +12278,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>173</v>
       </c>
@@ -12337,7 +12337,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>175</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>178</v>
       </c>
@@ -12416,7 +12416,7 @@
         <v>64</v>
       </c>
       <c r="G98" t="s">
-        <v>1910</v>
+        <v>20</v>
       </c>
       <c r="H98" t="s">
         <v>51</v>
@@ -12455,7 +12455,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>174</v>
       </c>
@@ -12504,7 +12504,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="2"/>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>1474</v>
       </c>
@@ -12563,7 +12563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>706</v>
       </c>
@@ -12622,7 +12622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>707</v>
       </c>
@@ -12681,7 +12681,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>1868</v>
       </c>
@@ -12740,7 +12740,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>1001</v>
       </c>
@@ -12799,7 +12799,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>1006</v>
       </c>
@@ -12846,7 +12846,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>1529</v>
       </c>
@@ -12905,7 +12905,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1520</v>
       </c>
@@ -12964,7 +12964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>85</v>
       </c>
@@ -13023,7 +13023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>81</v>
       </c>
@@ -13082,7 +13082,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>1451</v>
       </c>
@@ -13141,7 +13141,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>1450</v>
       </c>
@@ -13188,7 +13188,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>1453</v>
       </c>
@@ -13247,7 +13247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>1457</v>
       </c>
@@ -13306,7 +13306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>995</v>
       </c>
@@ -13365,7 +13365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1664</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>1656</v>
       </c>
@@ -13471,7 +13471,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>60</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>1601</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>1604</v>
       </c>
@@ -13636,7 +13636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>192</v>
       </c>
@@ -13695,7 +13695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>953</v>
       </c>
@@ -13744,7 +13744,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="2"/>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>20</v>
       </c>
@@ -13803,7 +13803,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>800</v>
       </c>
@@ -13850,7 +13850,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>797</v>
       </c>
@@ -13909,7 +13909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>1444</v>
       </c>
@@ -13968,7 +13968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>537</v>
       </c>
@@ -14015,7 +14015,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>13</v>
       </c>
@@ -14077,7 +14077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>12</v>
       </c>
@@ -14139,7 +14139,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>1769</v>
       </c>
@@ -14198,7 +14198,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>1627</v>
       </c>
@@ -14257,7 +14257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>506</v>
       </c>
@@ -14306,7 +14306,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="2"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>1463</v>
       </c>
@@ -14365,7 +14365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>651</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>650</v>
       </c>
@@ -14483,7 +14483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>656</v>
       </c>
@@ -14542,7 +14542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>693</v>
       </c>
@@ -14601,7 +14601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>694</v>
       </c>
@@ -14650,7 +14650,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="2"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>310</v>
       </c>
@@ -14709,7 +14709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>1145</v>
       </c>
@@ -14768,7 +14768,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>838</v>
       </c>
@@ -14827,7 +14827,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>1744</v>
       </c>
@@ -14886,7 +14886,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>611</v>
       </c>
@@ -14945,7 +14945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>316</v>
       </c>
@@ -15004,7 +15004,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>719</v>
       </c>
@@ -15053,7 +15053,7 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="2"/>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>275</v>
       </c>
@@ -15112,7 +15112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>167</v>
       </c>
@@ -15171,7 +15171,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>490</v>
       </c>
@@ -15220,7 +15220,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="2"/>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>205</v>
       </c>
@@ -15269,7 +15269,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="2"/>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>206</v>
       </c>
@@ -15328,7 +15328,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>765</v>
       </c>
@@ -15387,7 +15387,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>810</v>
       </c>
@@ -15446,7 +15446,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>803</v>
       </c>
@@ -15505,7 +15505,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>807</v>
       </c>
@@ -15564,7 +15564,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>814</v>
       </c>
@@ -15623,7 +15623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>813</v>
       </c>
@@ -15682,7 +15682,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>1536</v>
       </c>
@@ -15741,7 +15741,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>663</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>665</v>
       </c>
@@ -15849,7 +15849,7 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="2"/>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>499</v>
       </c>
@@ -15898,7 +15898,7 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="2"/>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>501</v>
       </c>
@@ -15957,7 +15957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>269</v>
       </c>
@@ -16016,7 +16016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>535</v>
       </c>
@@ -16078,7 +16078,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>363</v>
       </c>
@@ -16137,7 +16137,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>265</v>
       </c>
@@ -16196,7 +16196,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>241</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>1231</v>
       </c>
@@ -16314,7 +16314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>442</v>
       </c>
@@ -16373,7 +16373,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>123</v>
       </c>
@@ -16435,7 +16435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>128</v>
       </c>
@@ -16494,7 +16494,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>124</v>
       </c>
@@ -16553,7 +16553,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>1317</v>
       </c>
@@ -16612,7 +16612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>1313</v>
       </c>
@@ -16671,7 +16671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>1290</v>
       </c>
@@ -16730,7 +16730,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>1300</v>
       </c>
@@ -16789,7 +16789,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>1294</v>
       </c>
@@ -16838,7 +16838,7 @@
       <c r="Q175" s="1"/>
       <c r="R175" s="2"/>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>935</v>
       </c>
@@ -16897,7 +16897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>938</v>
       </c>
@@ -16956,7 +16956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>1689</v>
       </c>
@@ -17015,7 +17015,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>1103</v>
       </c>
@@ -17074,7 +17074,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>408</v>
       </c>
@@ -17136,7 +17136,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>1592</v>
       </c>
@@ -17195,7 +17195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>278</v>
       </c>
@@ -17254,7 +17254,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>280</v>
       </c>
@@ -17316,7 +17316,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>279</v>
       </c>
@@ -17375,7 +17375,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>720</v>
       </c>
@@ -17434,7 +17434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>722</v>
       </c>
@@ -17493,7 +17493,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>721</v>
       </c>
@@ -17552,7 +17552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>697</v>
       </c>
@@ -17599,7 +17599,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>705</v>
       </c>
@@ -17658,7 +17658,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>285</v>
       </c>
@@ -17717,7 +17717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>218</v>
       </c>
@@ -17776,7 +17776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>1899</v>
       </c>
@@ -17835,7 +17835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>443</v>
       </c>
@@ -17894,7 +17894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>321</v>
       </c>
@@ -17953,7 +17953,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>615</v>
       </c>
@@ -18012,7 +18012,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>619</v>
       </c>
@@ -18071,7 +18071,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>1469</v>
       </c>
@@ -18130,7 +18130,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>1466</v>
       </c>
@@ -18189,7 +18189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>423</v>
       </c>
@@ -18248,7 +18248,7 @@
         <v>1819</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>417</v>
       </c>
@@ -18295,7 +18295,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>914</v>
       </c>
@@ -18342,7 +18342,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>416</v>
       </c>
@@ -18401,7 +18401,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>100</v>
       </c>
@@ -18460,7 +18460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>234</v>
       </c>
@@ -18519,7 +18519,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>1254</v>
       </c>
@@ -18566,7 +18566,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>1123</v>
       </c>
@@ -18625,7 +18625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>360</v>
       </c>
@@ -18684,7 +18684,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>331</v>
       </c>
@@ -18743,7 +18743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>335</v>
       </c>
@@ -18802,7 +18802,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>1779</v>
       </c>
@@ -18861,7 +18861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>1775</v>
       </c>
@@ -18920,7 +18920,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>842</v>
       </c>
@@ -18982,7 +18982,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>698</v>
       </c>
@@ -19041,7 +19041,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>158</v>
       </c>
@@ -19100,7 +19100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>534</v>
       </c>
@@ -19147,7 +19147,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>96</v>
       </c>
@@ -19206,7 +19206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>16</v>
       </c>
@@ -19265,7 +19265,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>1025</v>
       </c>
@@ -19324,7 +19324,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>1019</v>
       </c>
@@ -19383,7 +19383,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>1037</v>
       </c>
@@ -19442,7 +19442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>1262</v>
       </c>
@@ -19501,7 +19501,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>1261</v>
       </c>
@@ -19560,7 +19560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>1876</v>
       </c>
@@ -19619,7 +19619,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>1880</v>
       </c>
@@ -19678,7 +19678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>1877</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>1878</v>
       </c>
@@ -19796,7 +19796,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>1756</v>
       </c>
@@ -19843,7 +19843,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>1195</v>
       </c>
@@ -19902,7 +19902,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>1159</v>
       </c>
@@ -19961,7 +19961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>1153</v>
       </c>
@@ -20008,7 +20008,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>1149</v>
       </c>
@@ -20067,7 +20067,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="232" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>1162</v>
       </c>
@@ -20126,7 +20126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>764</v>
       </c>
@@ -20185,7 +20185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>677</v>
       </c>
@@ -20244,7 +20244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>1733</v>
       </c>
@@ -20303,7 +20303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>724</v>
       </c>
@@ -20362,7 +20362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>1852</v>
       </c>
@@ -20409,7 +20409,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>1701</v>
       </c>
@@ -20468,7 +20468,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>669</v>
       </c>
@@ -20527,7 +20527,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>1838</v>
       </c>
@@ -20589,7 +20589,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="241" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>1831</v>
       </c>
@@ -20648,7 +20648,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="242" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>1678</v>
       </c>
@@ -20707,7 +20707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>1677</v>
       </c>
@@ -20766,7 +20766,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="244" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>1681</v>
       </c>
@@ -20825,7 +20825,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="245" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>1669</v>
       </c>
@@ -20884,7 +20884,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="246" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>1094</v>
       </c>
@@ -20931,7 +20931,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>1101</v>
       </c>
@@ -20990,7 +20990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>1800</v>
       </c>
@@ -21049,7 +21049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="249" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>1790</v>
       </c>
@@ -21108,7 +21108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>933</v>
       </c>
@@ -21167,7 +21167,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>44</v>
       </c>
@@ -21226,7 +21226,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="252" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>742</v>
       </c>
@@ -21285,7 +21285,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="253" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>746</v>
       </c>
@@ -21344,7 +21344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="254" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>741</v>
       </c>
@@ -21403,7 +21403,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="255" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>330</v>
       </c>
@@ -21462,7 +21462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="256" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>327</v>
       </c>
@@ -21509,7 +21509,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="257" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>324</v>
       </c>
@@ -21568,7 +21568,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="258" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>627</v>
       </c>
@@ -21627,7 +21627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="259" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>493</v>
       </c>
@@ -21686,7 +21686,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="260" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>120</v>
       </c>
@@ -21745,7 +21745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="261" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>431</v>
       </c>
@@ -21804,7 +21804,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="262" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>428</v>
       </c>
@@ -21863,7 +21863,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="263" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>1557</v>
       </c>
@@ -21922,7 +21922,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="264" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>1430</v>
       </c>
@@ -21981,7 +21981,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="265" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>1509</v>
       </c>
@@ -22040,7 +22040,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="266" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>1500</v>
       </c>
@@ -22099,7 +22099,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="267" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>548</v>
       </c>
@@ -22146,7 +22146,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="268" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>547</v>
       </c>
@@ -22205,7 +22205,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="269" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>544</v>
       </c>
@@ -22252,7 +22252,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="270" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>549</v>
       </c>
@@ -22311,7 +22311,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="271" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>690</v>
       </c>
@@ -22370,7 +22370,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>1274</v>
       </c>
@@ -22429,7 +22429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="273" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>1282</v>
       </c>
@@ -22488,7 +22488,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>1818</v>
       </c>
@@ -22547,7 +22547,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="275" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>497</v>
       </c>
@@ -22596,7 +22596,7 @@
       <c r="Q275" s="1"/>
       <c r="R275" s="2"/>
     </row>
-    <row r="276" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>613</v>
       </c>
@@ -22655,7 +22655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="277" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>1893</v>
       </c>
@@ -22714,7 +22714,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="278" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>1894</v>
       </c>
@@ -22773,7 +22773,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="279" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>1720</v>
       </c>
@@ -22832,7 +22832,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="280" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>1725</v>
       </c>
@@ -22891,7 +22891,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="281" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>1715</v>
       </c>
@@ -22950,7 +22950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="282" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>472</v>
       </c>
@@ -23012,7 +23012,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="283" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>469</v>
       </c>
@@ -23074,7 +23074,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="284" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>682</v>
       </c>
@@ -23133,7 +23133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="285" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>684</v>
       </c>
@@ -23192,7 +23192,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="286" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>686</v>
       </c>
@@ -23251,7 +23251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="287" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>115</v>
       </c>
@@ -23310,7 +23310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="288" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>116</v>
       </c>
@@ -23359,7 +23359,7 @@
       <c r="Q288" s="1"/>
       <c r="R288" s="2"/>
     </row>
-    <row r="289" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>1119</v>
       </c>
@@ -23418,7 +23418,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>1116</v>
       </c>
@@ -23477,7 +23477,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="291" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>514</v>
       </c>
@@ -23526,7 +23526,7 @@
       <c r="Q291" s="1"/>
       <c r="R291" s="2"/>
     </row>
-    <row r="292" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>1137</v>
       </c>
@@ -23585,7 +23585,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="293" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>1131</v>
       </c>
@@ -23644,7 +23644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="294" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>961</v>
       </c>
@@ -23703,7 +23703,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="295" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>660</v>
       </c>
@@ -23762,7 +23762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>661</v>
       </c>
@@ -23821,7 +23821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>898</v>
       </c>
@@ -23880,7 +23880,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="298" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>887</v>
       </c>
@@ -23939,7 +23939,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="299" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>901</v>
       </c>
@@ -23986,7 +23986,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="300" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>1104</v>
       </c>
@@ -24045,7 +24045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="301" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>662</v>
       </c>
@@ -24104,7 +24104,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>288</v>
       </c>
@@ -24163,7 +24163,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>286</v>
       </c>
@@ -24222,7 +24222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="304" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>195</v>
       </c>
@@ -24281,7 +24281,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="305" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>201</v>
       </c>
@@ -24340,7 +24340,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="306" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>79</v>
       </c>
@@ -24399,7 +24399,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="307" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>1807</v>
       </c>
@@ -24448,7 +24448,7 @@
       <c r="Q307" s="1"/>
       <c r="R307" s="2"/>
     </row>
-    <row r="308" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>78</v>
       </c>
@@ -24507,7 +24507,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="309" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>1434</v>
       </c>
@@ -24566,7 +24566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="310" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>259</v>
       </c>
@@ -24625,7 +24625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="311" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>246</v>
       </c>
@@ -24684,7 +24684,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="312" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>579</v>
       </c>
@@ -24733,7 +24733,7 @@
       <c r="Q312" s="1"/>
       <c r="R312" s="2"/>
     </row>
-    <row r="313" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>581</v>
       </c>
@@ -24782,7 +24782,7 @@
       <c r="Q313" s="1"/>
       <c r="R313" s="2"/>
     </row>
-    <row r="314" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>882</v>
       </c>
@@ -24831,7 +24831,7 @@
       <c r="Q314" s="1"/>
       <c r="R314" s="2"/>
     </row>
-    <row r="315" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>871</v>
       </c>
@@ -24893,7 +24893,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="316" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>602</v>
       </c>
@@ -24952,7 +24952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="317" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A317">
         <v>1543</v>
       </c>
@@ -25011,7 +25011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="318" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A318">
         <v>569</v>
       </c>
@@ -25058,7 +25058,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="319" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A319">
         <v>560</v>
       </c>
@@ -25117,7 +25117,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="320" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A320">
         <v>577</v>
       </c>
@@ -25176,7 +25176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="321" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A321">
         <v>567</v>
       </c>
@@ -25238,7 +25238,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="322" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A322">
         <v>575</v>
       </c>
@@ -25285,7 +25285,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="323" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A323">
         <v>555</v>
       </c>
@@ -25332,7 +25332,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="324" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A324">
         <v>559</v>
       </c>
@@ -25379,7 +25379,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="325" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A325">
         <v>573</v>
       </c>
@@ -25426,7 +25426,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="326" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A326">
         <v>564</v>
       </c>
@@ -25473,7 +25473,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="327" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A327">
         <v>563</v>
       </c>
@@ -25532,7 +25532,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="328" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A328">
         <v>145</v>
       </c>
@@ -25591,7 +25591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="329" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A329">
         <v>151</v>
       </c>
@@ -25650,7 +25650,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="330" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A330">
         <v>149</v>
       </c>
@@ -25709,7 +25709,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="331" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A331">
         <v>984</v>
       </c>
@@ -25768,7 +25768,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="332" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A332">
         <v>1711</v>
       </c>
@@ -25827,7 +25827,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="333" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A333">
         <v>1238</v>
       </c>
@@ -25886,7 +25886,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="334" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A334">
         <v>596</v>
       </c>
@@ -25935,7 +25935,7 @@
       <c r="Q334" s="1"/>
       <c r="R334" s="2"/>
     </row>
-    <row r="335" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A335">
         <v>590</v>
       </c>
@@ -25982,7 +25982,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="336" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A336">
         <v>591</v>
       </c>
@@ -26041,7 +26041,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="337" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A337">
         <v>1249</v>
       </c>
@@ -26100,7 +26100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="338" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A338">
         <v>1330</v>
       </c>
@@ -26159,7 +26159,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A339">
         <v>24</v>
       </c>
@@ -26218,7 +26218,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A340">
         <v>284</v>
       </c>
@@ -26277,7 +26277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="341" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A341">
         <v>1644</v>
       </c>
@@ -26336,7 +26336,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="342" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A342">
         <v>1635</v>
       </c>
@@ -26395,7 +26395,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="343" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A343">
         <v>1639</v>
       </c>
@@ -26454,7 +26454,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="344" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A344">
         <v>319</v>
       </c>
@@ -26513,7 +26513,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="345" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A345">
         <v>171</v>
       </c>
@@ -26572,7 +26572,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="346" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A346">
         <v>1355</v>
       </c>
@@ -26631,7 +26631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="347" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A347">
         <v>1360</v>
       </c>
@@ -26690,7 +26690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="348" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A348">
         <v>1374</v>
       </c>
@@ -26749,7 +26749,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="349" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A349">
         <v>983</v>
       </c>
@@ -26808,7 +26808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="350" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A350">
         <v>1321</v>
       </c>
@@ -26867,7 +26867,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="351" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A351">
         <v>30</v>
       </c>
@@ -26926,7 +26926,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="352" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A352">
         <v>1553</v>
       </c>
@@ -26985,7 +26985,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="353" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A353">
         <v>1788</v>
       </c>
@@ -27034,7 +27034,7 @@
       <c r="Q353" s="1"/>
       <c r="R353" s="2"/>
     </row>
-    <row r="354" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A354">
         <v>398</v>
       </c>
@@ -27083,7 +27083,7 @@
       <c r="Q354" s="1"/>
       <c r="R354" s="2"/>
     </row>
-    <row r="355" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A355">
         <v>394</v>
       </c>
@@ -27130,7 +27130,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="356" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A356">
         <v>395</v>
       </c>
@@ -27189,7 +27189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="357" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A357">
         <v>396</v>
       </c>
@@ -27248,7 +27248,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="358" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A358">
         <v>456</v>
       </c>
@@ -27307,7 +27307,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="359" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A359">
         <v>434</v>
       </c>
@@ -27366,7 +27366,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="360" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A360">
         <v>41</v>
       </c>
@@ -27425,7 +27425,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="361" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A361">
         <v>392</v>
       </c>
@@ -27472,7 +27472,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="362" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A362">
         <v>1573</v>
       </c>
@@ -27531,7 +27531,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="363" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A363">
         <v>91</v>
       </c>
@@ -27590,7 +27590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="364" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A364">
         <v>1705</v>
       </c>
@@ -27649,7 +27649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="365" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A365">
         <v>1928</v>
       </c>
@@ -27708,7 +27708,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="366" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A366">
         <v>674</v>
       </c>
@@ -27755,7 +27755,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="367" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A367">
         <v>672</v>
       </c>
@@ -27814,7 +27814,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="368" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A368">
         <v>670</v>
       </c>
@@ -27873,7 +27873,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="369" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A369">
         <v>1692</v>
       </c>
@@ -27932,7 +27932,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="370" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A370">
         <v>64</v>
       </c>
@@ -27991,7 +27991,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="371" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A371">
         <v>61</v>
       </c>
@@ -28050,7 +28050,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="372" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A372">
         <v>76</v>
       </c>
@@ -28109,7 +28109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="373" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A373">
         <v>1812</v>
       </c>
@@ -28168,7 +28168,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="374" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A374">
         <v>521</v>
       </c>
@@ -28215,7 +28215,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="375" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A375">
         <v>524</v>
       </c>
@@ -28277,7 +28277,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="376" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A376">
         <v>517</v>
       </c>
@@ -28324,7 +28324,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="377" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A377">
         <v>518</v>
       </c>
@@ -28386,7 +28386,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="378" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A378">
         <v>519</v>
       </c>
@@ -28433,7 +28433,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="379" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A379">
         <v>463</v>
       </c>
@@ -28492,7 +28492,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="380" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A380">
         <v>465</v>
       </c>
@@ -28551,7 +28551,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="381" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A381">
         <v>658</v>
       </c>
@@ -28610,7 +28610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="382" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A382">
         <v>659</v>
       </c>
@@ -28669,7 +28669,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="383" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A383">
         <v>782</v>
       </c>
@@ -28728,7 +28728,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="384" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A384">
         <v>793</v>
       </c>
@@ -28787,7 +28787,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="385" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A385">
         <v>789</v>
       </c>
@@ -28846,7 +28846,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="386" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A386">
         <v>785</v>
       </c>
@@ -28905,7 +28905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="387" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A387">
         <v>1753</v>
       </c>
@@ -28964,7 +28964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="388" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A388">
         <v>267</v>
       </c>
@@ -29011,7 +29011,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="389" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A389">
         <v>948</v>
       </c>
@@ -29070,7 +29070,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="390" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A390">
         <v>943</v>
       </c>
@@ -29129,7 +29129,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="391" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A391">
         <v>369</v>
       </c>
@@ -29188,7 +29188,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="392" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A392">
         <v>371</v>
       </c>
@@ -29235,7 +29235,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="393" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A393">
         <v>376</v>
       </c>
@@ -29294,7 +29294,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="394" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A394">
         <v>370</v>
       </c>
@@ -29341,7 +29341,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="395" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A395">
         <v>373</v>
       </c>
@@ -29400,7 +29400,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="396" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A396">
         <v>377</v>
       </c>
@@ -29459,7 +29459,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="397" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A397">
         <v>1966</v>
       </c>
@@ -29518,7 +29518,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="398" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A398">
         <v>382</v>
       </c>
@@ -29577,7 +29577,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="399" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A399">
         <v>384</v>
       </c>
@@ -29636,7 +29636,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="400" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A400">
         <v>390</v>
       </c>
@@ -29695,7 +29695,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="401" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A401">
         <v>385</v>
       </c>
@@ -29754,7 +29754,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="402" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A402">
         <v>391</v>
       </c>
@@ -29803,7 +29803,7 @@
       <c r="Q402" s="1"/>
       <c r="R402" s="2"/>
     </row>
-    <row r="403" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A403">
         <v>735</v>
       </c>
@@ -29862,7 +29862,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="404" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A404">
         <v>726</v>
       </c>
@@ -29921,7 +29921,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="405" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A405">
         <v>730</v>
       </c>
@@ -29980,7 +29980,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="406" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A406">
         <v>728</v>
       </c>
@@ -30039,7 +30039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="407" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A407">
         <v>313</v>
       </c>
@@ -30098,7 +30098,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="408" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A408">
         <v>312</v>
       </c>
@@ -30145,7 +30145,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="409" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A409">
         <v>366</v>
       </c>
@@ -30204,7 +30204,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="410" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A410">
         <v>249</v>
       </c>
@@ -30263,7 +30263,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="411" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A411">
         <v>251</v>
       </c>
@@ -30322,7 +30322,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="412" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A412">
         <v>1960</v>
       </c>
@@ -30381,7 +30381,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="413" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A413">
         <v>1915</v>
       </c>
@@ -30440,67 +30440,67 @@
         <v>27</v>
       </c>
     </row>
-    <row r="414" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E414"/>
     </row>
-    <row r="415" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E415"/>
     </row>
-    <row r="416" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E416"/>
     </row>
-    <row r="417" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E417"/>
     </row>
-    <row r="418" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E418"/>
     </row>
-    <row r="419" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E419"/>
     </row>
-    <row r="420" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E420"/>
     </row>
-    <row r="421" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E421"/>
     </row>
-    <row r="422" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E422"/>
     </row>
-    <row r="423" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E423"/>
     </row>
-    <row r="424" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E424"/>
     </row>
-    <row r="425" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E425"/>
     </row>
-    <row r="426" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E426"/>
     </row>
-    <row r="427" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E427"/>
     </row>
-    <row r="428" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E428"/>
     </row>
-    <row r="429" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E429"/>
     </row>
-    <row r="430" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E430"/>
     </row>
-    <row r="431" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E431"/>
     </row>
-    <row r="432" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E432"/>
     </row>
-    <row r="433" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E433"/>
     </row>
-    <row r="434" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E434"/>
     </row>
   </sheetData>
@@ -30735,29 +30735,29 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.7265625" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -30819,7 +30819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>1949</v>
       </c>
@@ -30871,7 +30871,7 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1950</v>
       </c>
@@ -30933,7 +30933,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>1951</v>
       </c>
@@ -30995,7 +30995,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -31017,7 +31017,7 @@
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>1725</v>
       </c>
@@ -31058,7 +31058,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>1726</v>
       </c>
@@ -31102,7 +31102,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>1727</v>
       </c>
@@ -31143,7 +31143,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>1728</v>
       </c>
@@ -31184,7 +31184,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>1729</v>
       </c>
@@ -31225,7 +31225,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>1730</v>
       </c>
@@ -31266,7 +31266,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>1731</v>
       </c>
@@ -31307,7 +31307,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>1732</v>
       </c>
@@ -31351,7 +31351,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>1733</v>
       </c>
@@ -31395,7 +31395,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>1734</v>
       </c>
@@ -31436,7 +31436,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>1735</v>
       </c>
@@ -31477,7 +31477,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>1765</v>
       </c>
@@ -31518,7 +31518,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>1766</v>
       </c>
@@ -31559,7 +31559,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>1767</v>
       </c>
@@ -31600,7 +31600,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>1768</v>
       </c>
@@ -31641,7 +31641,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>1769</v>
       </c>
@@ -31682,7 +31682,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>1784</v>
       </c>
@@ -31723,7 +31723,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>1785</v>
       </c>
@@ -31764,7 +31764,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>1788</v>
       </c>
@@ -31808,7 +31808,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>1789</v>
       </c>
@@ -31852,12 +31852,12 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>1736</v>
       </c>
@@ -31901,7 +31901,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>1737</v>
       </c>
@@ -31945,7 +31945,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>1738</v>
       </c>
@@ -31989,7 +31989,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>1739</v>
       </c>
@@ -32033,7 +32033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E33" s="10"/>
     </row>
   </sheetData>
@@ -32055,16 +32055,16 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>1948</v>
       </c>
@@ -32108,13 +32108,13 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B10" ca="1" si="0">SUMPRODUCT(COUNTIF(INDIRECT("'"&amp;$A$16:$A$17&amp;"'!G:G"),A2))</f>
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D2" t="s">
         <v>1684</v>
@@ -32159,7 +32159,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1762</v>
       </c>
@@ -32210,7 +32210,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -32261,7 +32261,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1643</v>
       </c>
@@ -32312,7 +32312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1686</v>
       </c>
@@ -32344,7 +32344,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>1763</v>
       </c>
@@ -32388,7 +32388,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>1672</v>
       </c>
@@ -32425,7 +32425,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1742</v>
       </c>
@@ -32441,7 +32441,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -32464,20 +32464,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="D11" t="s">
         <v>1910</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
         <v>1764</v>
       </c>
       <c r="B12" s="12">
         <f ca="1">B2+B4+B10</f>
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>1933</v>
@@ -32487,28 +32487,28 @@
         <v>412</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
         <v>1656</v>
       </c>
       <c r="B13" s="12">
         <f ca="1">SUM(B2:B10)</f>
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>1759</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1760</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1761</v>
       </c>
@@ -32532,29 +32532,29 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.7265625" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -32616,7 +32616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1956</v>
       </c>
@@ -32657,7 +32657,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>289</v>
       </c>
@@ -32698,7 +32698,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>1696</v>
       </c>

</xml_diff>

<commit_message>
couple of eBird additions
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD63533-95C3-4F46-BC1D-99C5B726A50E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3BDE16-7E88-4A30-B355-E11A5FD983D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11630" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7355" uniqueCount="1968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7363" uniqueCount="1976">
   <si>
     <t>Taxon Sort</t>
   </si>
@@ -6154,6 +6154,30 @@
   </si>
   <si>
     <t>no photo or audio of potential wild birds on eBird; two at Anstead on 4th Sep 2010 maybe good candidates for vagrants? Sue Lee 13/03/19 Very good candidate for vagrants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article </t>
+  </si>
+  <si>
+    <t>306_Oriental Plover_Sunbird25(4)</t>
+  </si>
+  <si>
+    <t>https://search.informit.com.au/documentSummary;dn=209368307262145;res=IELHSS</t>
+  </si>
+  <si>
+    <t>Archerfield Airport</t>
+  </si>
+  <si>
+    <t>490_Little Penguin_Emu55(1)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1071/MU955072a</t>
+  </si>
+  <si>
+    <t>Moreton Bay Mouth</t>
+  </si>
+  <si>
+    <t>Con Reilly</t>
   </si>
 </sst>
 </file>
@@ -6745,9 +6769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787458D5-0D53-4EB5-974E-BD980B126E90}">
   <dimension ref="A1:T435"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11584,7 +11608,7 @@
         <v>499</v>
       </c>
       <c r="G83" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="H83" t="s">
         <v>499</v>
@@ -11596,7 +11620,7 @@
         <v>499</v>
       </c>
       <c r="K83" t="s">
-        <v>108</v>
+        <v>1683</v>
       </c>
       <c r="L83" t="s">
         <v>1684</v>
@@ -11608,10 +11632,23 @@
         <v>409</v>
       </c>
       <c r="O83" t="s">
-        <v>1839</v>
-      </c>
-      <c r="Q83" s="1"/>
-      <c r="R83" s="2"/>
+        <v>1968</v>
+      </c>
+      <c r="P83" t="s">
+        <v>1969</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="R83" s="2">
+        <v>34651</v>
+      </c>
+      <c r="S83" t="s">
+        <v>1971</v>
+      </c>
+      <c r="T83" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A84">
@@ -14208,7 +14245,7 @@
         <v>499</v>
       </c>
       <c r="K129" t="s">
-        <v>108</v>
+        <v>1683</v>
       </c>
       <c r="L129" t="s">
         <v>1684</v>
@@ -15269,10 +15306,23 @@
         <v>1897</v>
       </c>
       <c r="O147" t="s">
-        <v>1839</v>
-      </c>
-      <c r="Q147" s="1"/>
-      <c r="R147" s="2"/>
+        <v>1968</v>
+      </c>
+      <c r="P147" t="s">
+        <v>1972</v>
+      </c>
+      <c r="Q147" s="1" t="s">
+        <v>1973</v>
+      </c>
+      <c r="R147" s="2">
+        <v>19633</v>
+      </c>
+      <c r="S147" t="s">
+        <v>1974</v>
+      </c>
+      <c r="T147" t="s">
+        <v>1975</v>
+      </c>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A148">
@@ -30778,7 +30828,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32046,7 +32096,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32108,14 +32158,14 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B10" ca="1" si="0">SUMPRODUCT(COUNTIF(INDIRECT("'"&amp;$A$16:$A$17&amp;"'!G:G"),A2))</f>
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D2" t="s">
         <v>1683</v>
       </c>
       <c r="E2">
         <f ca="1">SUMPRODUCT(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!K:K"),D2))</f>
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>23</v>
@@ -32268,7 +32318,7 @@
       </c>
       <c r="E5">
         <f ca="1">SUMPRODUCT(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!K:K"),D5))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>1839</v>
@@ -32351,7 +32401,7 @@
       </c>
       <c r="E7" s="12">
         <f ca="1">E2+E4</f>
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>1932</v>
@@ -32441,7 +32491,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>1932</v>

</xml_diff>

<commit_message>
update species common names to conform to eBird Aus
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3BDE16-7E88-4A30-B355-E11A5FD983D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9C627E-8586-4627-96D8-078F1B346008}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11630" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB - Primary List" sheetId="1" r:id="rId1"/>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7363" uniqueCount="1976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7363" uniqueCount="1977">
   <si>
     <t>Taxon Sort</t>
   </si>
@@ -6178,6 +6178,9 @@
   </si>
   <si>
     <t>Con Reilly</t>
+  </si>
+  <si>
+    <t>Double-eyed Fig-Parrot</t>
   </si>
 </sst>
 </file>
@@ -6769,39 +6772,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787458D5-0D53-4EB5-974E-BD980B126E90}">
   <dimension ref="A1:T435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A389" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D410" sqref="D410"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.1796875" customWidth="1"/>
-    <col min="14" max="14" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6863,7 +6866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -6925,7 +6928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -6987,7 +6990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -7049,7 +7052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16</v>
       </c>
@@ -7108,7 +7111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -7167,7 +7170,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>24</v>
       </c>
@@ -7226,7 +7229,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>28</v>
       </c>
@@ -7285,7 +7288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -7296,7 +7299,7 @@
         <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>63</v>
@@ -7344,7 +7347,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>34</v>
       </c>
@@ -7403,7 +7406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>36</v>
       </c>
@@ -7462,7 +7465,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>37</v>
       </c>
@@ -7521,7 +7524,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>41</v>
       </c>
@@ -7580,7 +7583,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>42</v>
       </c>
@@ -7639,7 +7642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43</v>
       </c>
@@ -7698,7 +7701,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>44</v>
       </c>
@@ -7757,7 +7760,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>47</v>
       </c>
@@ -7768,7 +7771,7 @@
         <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>103</v>
@@ -7816,7 +7819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>60</v>
       </c>
@@ -7863,7 +7866,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>61</v>
       </c>
@@ -7922,7 +7925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>64</v>
       </c>
@@ -7981,7 +7984,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>76</v>
       </c>
@@ -8040,7 +8043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>78</v>
       </c>
@@ -8099,7 +8102,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>79</v>
       </c>
@@ -8158,7 +8161,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>81</v>
       </c>
@@ -8169,7 +8172,7 @@
         <v>135</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>136</v>
@@ -8217,7 +8220,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>85</v>
       </c>
@@ -8276,7 +8279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>91</v>
       </c>
@@ -8335,7 +8338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>96</v>
       </c>
@@ -8394,7 +8397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>100</v>
       </c>
@@ -8453,7 +8456,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>115</v>
       </c>
@@ -8512,7 +8515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>116</v>
       </c>
@@ -8561,7 +8564,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>120</v>
       </c>
@@ -8620,7 +8623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>123</v>
       </c>
@@ -8682,7 +8685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>124</v>
       </c>
@@ -8741,7 +8744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>128</v>
       </c>
@@ -8800,7 +8803,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>134</v>
       </c>
@@ -8859,7 +8862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>145</v>
       </c>
@@ -8918,7 +8921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>149</v>
       </c>
@@ -8977,7 +8980,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>151</v>
       </c>
@@ -9036,7 +9039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>158</v>
       </c>
@@ -9095,7 +9098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>161</v>
       </c>
@@ -9154,7 +9157,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>167</v>
       </c>
@@ -9213,7 +9216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>171</v>
       </c>
@@ -9272,7 +9275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>173</v>
       </c>
@@ -9331,7 +9334,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>174</v>
       </c>
@@ -9380,7 +9383,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="2"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>175</v>
       </c>
@@ -9439,7 +9442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>178</v>
       </c>
@@ -9498,7 +9501,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>184</v>
       </c>
@@ -9557,7 +9560,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>186</v>
       </c>
@@ -9616,7 +9619,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>189</v>
       </c>
@@ -9675,7 +9678,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>192</v>
       </c>
@@ -9734,7 +9737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>195</v>
       </c>
@@ -9793,7 +9796,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>201</v>
       </c>
@@ -9852,7 +9855,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>205</v>
       </c>
@@ -9901,7 +9904,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="2"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>206</v>
       </c>
@@ -9960,7 +9963,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>213</v>
       </c>
@@ -10019,7 +10022,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>218</v>
       </c>
@@ -10078,7 +10081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>223</v>
       </c>
@@ -10122,7 +10125,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>228</v>
       </c>
@@ -10181,7 +10184,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>234</v>
       </c>
@@ -10240,7 +10243,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>241</v>
       </c>
@@ -10299,7 +10302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>246</v>
       </c>
@@ -10358,7 +10361,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>249</v>
       </c>
@@ -10417,7 +10420,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>251</v>
       </c>
@@ -10476,7 +10479,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>253</v>
       </c>
@@ -10535,7 +10538,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>259</v>
       </c>
@@ -10594,7 +10597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>265</v>
       </c>
@@ -10653,7 +10656,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>267</v>
       </c>
@@ -10700,7 +10703,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>269</v>
       </c>
@@ -10759,7 +10762,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>273</v>
       </c>
@@ -10818,7 +10821,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>274</v>
       </c>
@@ -10877,7 +10880,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>275</v>
       </c>
@@ -10936,7 +10939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>278</v>
       </c>
@@ -10995,7 +10998,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>279</v>
       </c>
@@ -11054,7 +11057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>280</v>
       </c>
@@ -11116,7 +11119,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>284</v>
       </c>
@@ -11175,7 +11178,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>285</v>
       </c>
@@ -11234,7 +11237,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>286</v>
       </c>
@@ -11293,7 +11296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>288</v>
       </c>
@@ -11352,7 +11355,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>297</v>
       </c>
@@ -11411,7 +11414,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>298</v>
       </c>
@@ -11470,7 +11473,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>300</v>
       </c>
@@ -11529,7 +11532,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>303</v>
       </c>
@@ -11588,7 +11591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>306</v>
       </c>
@@ -11650,7 +11653,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>310</v>
       </c>
@@ -11709,7 +11712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>312</v>
       </c>
@@ -11756,7 +11759,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>313</v>
       </c>
@@ -11815,7 +11818,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>316</v>
       </c>
@@ -11874,7 +11877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>319</v>
       </c>
@@ -11885,7 +11888,7 @@
         <v>425</v>
       </c>
       <c r="D88" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>426</v>
@@ -11933,7 +11936,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>321</v>
       </c>
@@ -11992,7 +11995,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>324</v>
       </c>
@@ -12051,7 +12054,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>327</v>
       </c>
@@ -12098,7 +12101,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>330</v>
       </c>
@@ -12157,7 +12160,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>331</v>
       </c>
@@ -12216,7 +12219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>335</v>
       </c>
@@ -12275,7 +12278,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>337</v>
       </c>
@@ -12334,7 +12337,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>339</v>
       </c>
@@ -12393,7 +12396,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>340</v>
       </c>
@@ -12452,7 +12455,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>343</v>
       </c>
@@ -12511,7 +12514,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>344</v>
       </c>
@@ -12570,7 +12573,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>346</v>
       </c>
@@ -12629,7 +12632,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>348</v>
       </c>
@@ -12688,7 +12691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>349</v>
       </c>
@@ -12747,7 +12750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>350</v>
       </c>
@@ -12806,7 +12809,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>351</v>
       </c>
@@ -12865,7 +12868,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>358</v>
       </c>
@@ -12924,7 +12927,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>359</v>
       </c>
@@ -12983,7 +12986,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>360</v>
       </c>
@@ -13042,7 +13045,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>363</v>
       </c>
@@ -13101,7 +13104,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>366</v>
       </c>
@@ -13160,7 +13163,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>367</v>
       </c>
@@ -13219,7 +13222,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>369</v>
       </c>
@@ -13278,7 +13281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>370</v>
       </c>
@@ -13325,7 +13328,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>371</v>
       </c>
@@ -13372,7 +13375,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>373</v>
       </c>
@@ -13431,7 +13434,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>376</v>
       </c>
@@ -13490,7 +13493,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>377</v>
       </c>
@@ -13549,7 +13552,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>382</v>
       </c>
@@ -13608,7 +13611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>384</v>
       </c>
@@ -13667,7 +13670,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>385</v>
       </c>
@@ -13726,7 +13729,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>390</v>
       </c>
@@ -13785,7 +13788,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>391</v>
       </c>
@@ -13834,7 +13837,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="2"/>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>392</v>
       </c>
@@ -13881,7 +13884,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>394</v>
       </c>
@@ -13928,7 +13931,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>395</v>
       </c>
@@ -13987,7 +13990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>396</v>
       </c>
@@ -14046,7 +14049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>398</v>
       </c>
@@ -14095,7 +14098,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="2"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>400</v>
       </c>
@@ -14154,7 +14157,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>404</v>
       </c>
@@ -14213,7 +14216,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>406</v>
       </c>
@@ -14224,7 +14227,7 @@
         <v>1857</v>
       </c>
       <c r="D129" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>1858</v>
@@ -14262,7 +14265,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="2"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>408</v>
       </c>
@@ -14324,7 +14327,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>411</v>
       </c>
@@ -14383,7 +14386,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>416</v>
       </c>
@@ -14442,7 +14445,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>417</v>
       </c>
@@ -14489,7 +14492,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>423</v>
       </c>
@@ -14548,7 +14551,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>428</v>
       </c>
@@ -14607,7 +14610,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>431</v>
       </c>
@@ -14666,7 +14669,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>434</v>
       </c>
@@ -14725,7 +14728,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>442</v>
       </c>
@@ -14784,7 +14787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>443</v>
       </c>
@@ -14843,7 +14846,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>444</v>
       </c>
@@ -14902,7 +14905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>446</v>
       </c>
@@ -14961,7 +14964,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>456</v>
       </c>
@@ -15020,7 +15023,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>463</v>
       </c>
@@ -15079,7 +15082,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>465</v>
       </c>
@@ -15090,7 +15093,7 @@
         <v>635</v>
       </c>
       <c r="D144" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>636</v>
@@ -15138,7 +15141,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>469</v>
       </c>
@@ -15200,7 +15203,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>472</v>
       </c>
@@ -15262,7 +15265,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>490</v>
       </c>
@@ -15324,7 +15327,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>493</v>
       </c>
@@ -15383,7 +15386,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>497</v>
       </c>
@@ -15432,7 +15435,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="2"/>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>499</v>
       </c>
@@ -15481,7 +15484,7 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="2"/>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>501</v>
       </c>
@@ -15540,7 +15543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>506</v>
       </c>
@@ -15589,7 +15592,7 @@
       <c r="Q152" s="1"/>
       <c r="R152" s="2"/>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>514</v>
       </c>
@@ -15638,7 +15641,7 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="2"/>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>517</v>
       </c>
@@ -15685,7 +15688,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>518</v>
       </c>
@@ -15747,7 +15750,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>519</v>
       </c>
@@ -15794,7 +15797,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>521</v>
       </c>
@@ -15841,7 +15844,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>524</v>
       </c>
@@ -15903,7 +15906,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>534</v>
       </c>
@@ -15950,7 +15953,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>535</v>
       </c>
@@ -16012,7 +16015,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>537</v>
       </c>
@@ -16059,7 +16062,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>544</v>
       </c>
@@ -16106,7 +16109,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>547</v>
       </c>
@@ -16165,7 +16168,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>548</v>
       </c>
@@ -16212,7 +16215,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>549</v>
       </c>
@@ -16271,7 +16274,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>555</v>
       </c>
@@ -16318,7 +16321,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>559</v>
       </c>
@@ -16365,7 +16368,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>560</v>
       </c>
@@ -16424,7 +16427,7 @@
         <v>1693</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>563</v>
       </c>
@@ -16483,7 +16486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>564</v>
       </c>
@@ -16530,7 +16533,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>567</v>
       </c>
@@ -16592,7 +16595,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>569</v>
       </c>
@@ -16639,7 +16642,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>573</v>
       </c>
@@ -16686,7 +16689,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>575</v>
       </c>
@@ -16733,7 +16736,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>577</v>
       </c>
@@ -16792,7 +16795,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>579</v>
       </c>
@@ -16841,7 +16844,7 @@
       <c r="Q176" s="1"/>
       <c r="R176" s="2"/>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>581</v>
       </c>
@@ -16890,7 +16893,7 @@
       <c r="Q177" s="1"/>
       <c r="R177" s="2"/>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>582</v>
       </c>
@@ -16949,7 +16952,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>583</v>
       </c>
@@ -16998,7 +17001,7 @@
       <c r="Q179" s="1"/>
       <c r="R179" s="2"/>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>584</v>
       </c>
@@ -17057,7 +17060,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>587</v>
       </c>
@@ -17106,7 +17109,7 @@
       <c r="Q181" s="1"/>
       <c r="R181" s="2"/>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>589</v>
       </c>
@@ -17155,7 +17158,7 @@
       <c r="Q182" s="1"/>
       <c r="R182" s="2"/>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>590</v>
       </c>
@@ -17202,7 +17205,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>591</v>
       </c>
@@ -17261,7 +17264,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>596</v>
       </c>
@@ -17310,7 +17313,7 @@
       <c r="Q185" s="1"/>
       <c r="R185" s="2"/>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>602</v>
       </c>
@@ -17369,7 +17372,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>611</v>
       </c>
@@ -17428,7 +17431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>613</v>
       </c>
@@ -17487,7 +17490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>614</v>
       </c>
@@ -17549,7 +17552,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>615</v>
       </c>
@@ -17608,7 +17611,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>619</v>
       </c>
@@ -17667,7 +17670,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>627</v>
       </c>
@@ -17726,7 +17729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>629</v>
       </c>
@@ -17785,7 +17788,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>636</v>
       </c>
@@ -17844,7 +17847,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>640</v>
       </c>
@@ -17903,7 +17906,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>645</v>
       </c>
@@ -17962,7 +17965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>647</v>
       </c>
@@ -18021,7 +18024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>650</v>
       </c>
@@ -18080,7 +18083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>651</v>
       </c>
@@ -18139,7 +18142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>656</v>
       </c>
@@ -18198,7 +18201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>658</v>
       </c>
@@ -18257,7 +18260,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>659</v>
       </c>
@@ -18316,7 +18319,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>660</v>
       </c>
@@ -18375,7 +18378,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>661</v>
       </c>
@@ -18434,7 +18437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>662</v>
       </c>
@@ -18493,7 +18496,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>663</v>
       </c>
@@ -18552,7 +18555,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>665</v>
       </c>
@@ -18601,7 +18604,7 @@
       <c r="Q207" s="1"/>
       <c r="R207" s="2"/>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>669</v>
       </c>
@@ -18660,7 +18663,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>670</v>
       </c>
@@ -18719,7 +18722,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>672</v>
       </c>
@@ -18778,7 +18781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>674</v>
       </c>
@@ -18825,7 +18828,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>677</v>
       </c>
@@ -18884,7 +18887,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="213" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>682</v>
       </c>
@@ -18943,7 +18946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="214" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>684</v>
       </c>
@@ -19002,7 +19005,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>686</v>
       </c>
@@ -19061,7 +19064,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="216" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>688</v>
       </c>
@@ -19120,7 +19123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>690</v>
       </c>
@@ -19179,7 +19182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>693</v>
       </c>
@@ -19238,7 +19241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>694</v>
       </c>
@@ -19287,7 +19290,7 @@
       <c r="Q219" s="1"/>
       <c r="R219" s="2"/>
     </row>
-    <row r="220" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>697</v>
       </c>
@@ -19334,7 +19337,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="221" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>698</v>
       </c>
@@ -19393,7 +19396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>699</v>
       </c>
@@ -19452,7 +19455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>702</v>
       </c>
@@ -19511,7 +19514,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="224" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>705</v>
       </c>
@@ -19570,7 +19573,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>706</v>
       </c>
@@ -19629,7 +19632,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>707</v>
       </c>
@@ -19688,7 +19691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>708</v>
       </c>
@@ -19747,7 +19750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>710</v>
       </c>
@@ -19806,7 +19809,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>717</v>
       </c>
@@ -19865,7 +19868,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>719</v>
       </c>
@@ -19914,7 +19917,7 @@
       <c r="Q230" s="1"/>
       <c r="R230" s="2"/>
     </row>
-    <row r="231" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>720</v>
       </c>
@@ -19973,7 +19976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="232" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>721</v>
       </c>
@@ -20032,7 +20035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="233" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>722</v>
       </c>
@@ -20091,7 +20094,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="234" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>724</v>
       </c>
@@ -20150,7 +20153,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>726</v>
       </c>
@@ -20209,7 +20212,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>728</v>
       </c>
@@ -20268,7 +20271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="237" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>730</v>
       </c>
@@ -20327,7 +20330,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>735</v>
       </c>
@@ -20386,7 +20389,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="239" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>741</v>
       </c>
@@ -20445,7 +20448,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="240" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>742</v>
       </c>
@@ -20504,7 +20507,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="241" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>746</v>
       </c>
@@ -20563,7 +20566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="242" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>764</v>
       </c>
@@ -20622,7 +20625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>765</v>
       </c>
@@ -20681,7 +20684,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="244" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>773</v>
       </c>
@@ -20740,7 +20743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="245" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>782</v>
       </c>
@@ -20799,7 +20802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="246" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>785</v>
       </c>
@@ -20858,7 +20861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="247" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>789</v>
       </c>
@@ -20917,7 +20920,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="248" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>793</v>
       </c>
@@ -20976,7 +20979,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="249" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>797</v>
       </c>
@@ -21035,7 +21038,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>800</v>
       </c>
@@ -21082,7 +21085,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="251" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>803</v>
       </c>
@@ -21093,7 +21096,7 @@
         <v>953</v>
       </c>
       <c r="D251" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E251" s="8" t="s">
         <v>954</v>
@@ -21141,7 +21144,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="252" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>807</v>
       </c>
@@ -21200,7 +21203,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="253" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>810</v>
       </c>
@@ -21259,7 +21262,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="254" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>813</v>
       </c>
@@ -21318,7 +21321,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="255" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>814</v>
       </c>
@@ -21377,7 +21380,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="256" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A256" s="7">
         <v>818</v>
       </c>
@@ -21426,7 +21429,7 @@
       <c r="Q256" s="1"/>
       <c r="R256" s="2"/>
     </row>
-    <row r="257" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>819</v>
       </c>
@@ -21473,7 +21476,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="258" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>825</v>
       </c>
@@ -21532,7 +21535,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="259" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>829</v>
       </c>
@@ -21591,7 +21594,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="260" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>838</v>
       </c>
@@ -21650,7 +21653,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="261" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>842</v>
       </c>
@@ -21712,7 +21715,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="262" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>845</v>
       </c>
@@ -21774,7 +21777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>849</v>
       </c>
@@ -21833,7 +21836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="264" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>853</v>
       </c>
@@ -21892,7 +21895,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="265" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>861</v>
       </c>
@@ -21951,7 +21954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="266" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>864</v>
       </c>
@@ -21998,7 +22001,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="267" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>871</v>
       </c>
@@ -22060,7 +22063,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="268" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>882</v>
       </c>
@@ -22109,7 +22112,7 @@
       <c r="Q268" s="1"/>
       <c r="R268" s="2"/>
     </row>
-    <row r="269" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>887</v>
       </c>
@@ -22168,7 +22171,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="270" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>898</v>
       </c>
@@ -22227,7 +22230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="271" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>901</v>
       </c>
@@ -22274,7 +22277,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="272" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>914</v>
       </c>
@@ -22321,7 +22324,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="273" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>933</v>
       </c>
@@ -22380,7 +22383,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="274" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>935</v>
       </c>
@@ -22439,7 +22442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>938</v>
       </c>
@@ -22498,7 +22501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="276" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>943</v>
       </c>
@@ -22557,7 +22560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="277" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>948</v>
       </c>
@@ -22616,7 +22619,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="278" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>953</v>
       </c>
@@ -22627,7 +22630,7 @@
         <v>1882</v>
       </c>
       <c r="D278" t="s">
-        <v>1881</v>
+        <v>1976</v>
       </c>
       <c r="E278" s="8" t="s">
         <v>1883</v>
@@ -22665,7 +22668,7 @@
       <c r="Q278" s="1"/>
       <c r="R278" s="2"/>
     </row>
-    <row r="279" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>961</v>
       </c>
@@ -22724,7 +22727,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="280" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>980</v>
       </c>
@@ -22783,7 +22786,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="281" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>983</v>
       </c>
@@ -22842,7 +22845,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="282" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>984</v>
       </c>
@@ -22901,7 +22904,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="283" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>995</v>
       </c>
@@ -22960,7 +22963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="284" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>1001</v>
       </c>
@@ -23019,7 +23022,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="285" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>1006</v>
       </c>
@@ -23066,7 +23069,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="286" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>1019</v>
       </c>
@@ -23125,7 +23128,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="287" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>1025</v>
       </c>
@@ -23184,7 +23187,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="288" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1037</v>
       </c>
@@ -23243,7 +23246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="289" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1094</v>
       </c>
@@ -23290,7 +23293,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="290" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>1101</v>
       </c>
@@ -23349,7 +23352,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="291" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1103</v>
       </c>
@@ -23408,7 +23411,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="292" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1104</v>
       </c>
@@ -23467,7 +23470,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="293" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1116</v>
       </c>
@@ -23526,7 +23529,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="294" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>1119</v>
       </c>
@@ -23585,7 +23588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="295" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>1123</v>
       </c>
@@ -23644,7 +23647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>1131</v>
       </c>
@@ -23703,7 +23706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>1137</v>
       </c>
@@ -23762,7 +23765,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="298" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1145</v>
       </c>
@@ -23821,7 +23824,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="299" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>1149</v>
       </c>
@@ -23880,7 +23883,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="300" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>1153</v>
       </c>
@@ -23927,7 +23930,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="301" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>1159</v>
       </c>
@@ -23986,7 +23989,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>1162</v>
       </c>
@@ -24045,7 +24048,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="303" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1171</v>
       </c>
@@ -24104,7 +24107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="304" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>1195</v>
       </c>
@@ -24163,7 +24166,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="305" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>1208</v>
       </c>
@@ -24222,7 +24225,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="306" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>1210</v>
       </c>
@@ -24281,7 +24284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="307" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>1214</v>
       </c>
@@ -24340,7 +24343,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="308" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>1215</v>
       </c>
@@ -24399,7 +24402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="309" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>1231</v>
       </c>
@@ -24458,7 +24461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="310" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>1238</v>
       </c>
@@ -24517,7 +24520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="311" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>1249</v>
       </c>
@@ -24576,7 +24579,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="312" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>1250</v>
       </c>
@@ -24635,7 +24638,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="313" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>1254</v>
       </c>
@@ -24682,7 +24685,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="314" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>1261</v>
       </c>
@@ -24741,7 +24744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="315" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>1262</v>
       </c>
@@ -24800,7 +24803,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="316" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>1274</v>
       </c>
@@ -24859,7 +24862,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="317" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>1282</v>
       </c>
@@ -24918,7 +24921,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="318" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>1290</v>
       </c>
@@ -24977,7 +24980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="319" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>1294</v>
       </c>
@@ -25026,7 +25029,7 @@
       <c r="Q319" s="1"/>
       <c r="R319" s="2"/>
     </row>
-    <row r="320" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>1300</v>
       </c>
@@ -25085,7 +25088,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="321" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>1313</v>
       </c>
@@ -25144,7 +25147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="322" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>1317</v>
       </c>
@@ -25203,7 +25206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="323" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>1321</v>
       </c>
@@ -25262,7 +25265,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="324" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>1330</v>
       </c>
@@ -25321,7 +25324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="325" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>1355</v>
       </c>
@@ -25380,7 +25383,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="326" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>1360</v>
       </c>
@@ -25439,7 +25442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="327" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>1374</v>
       </c>
@@ -25498,7 +25501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="328" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>1389</v>
       </c>
@@ -25557,7 +25560,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="329" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>1394</v>
       </c>
@@ -25619,7 +25622,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="330" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>1398</v>
       </c>
@@ -25678,7 +25681,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="331" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>1411</v>
       </c>
@@ -25737,7 +25740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="332" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>1424</v>
       </c>
@@ -25796,7 +25799,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="333" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>1430</v>
       </c>
@@ -25855,7 +25858,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="334" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>1434</v>
       </c>
@@ -25914,7 +25917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="335" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>1444</v>
       </c>
@@ -25973,7 +25976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="336" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>1450</v>
       </c>
@@ -26020,7 +26023,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="337" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>1451</v>
       </c>
@@ -26079,7 +26082,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="338" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>1453</v>
       </c>
@@ -26138,7 +26141,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>1457</v>
       </c>
@@ -26197,7 +26200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>1463</v>
       </c>
@@ -26256,7 +26259,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="341" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>1466</v>
       </c>
@@ -26315,7 +26318,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="342" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>1469</v>
       </c>
@@ -26374,7 +26377,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="343" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>1474</v>
       </c>
@@ -26433,7 +26436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="344" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>1500</v>
       </c>
@@ -26492,7 +26495,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="345" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>1509</v>
       </c>
@@ -26551,7 +26554,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="346" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>1520</v>
       </c>
@@ -26610,7 +26613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="347" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>1529</v>
       </c>
@@ -26669,7 +26672,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="348" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>1536</v>
       </c>
@@ -26728,7 +26731,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="349" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>1543</v>
       </c>
@@ -26787,7 +26790,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="350" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>1553</v>
       </c>
@@ -26846,7 +26849,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="351" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>1557</v>
       </c>
@@ -26905,7 +26908,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="352" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>1573</v>
       </c>
@@ -26964,7 +26967,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="353" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>1592</v>
       </c>
@@ -27023,7 +27026,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="354" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>1601</v>
       </c>
@@ -27082,7 +27085,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="355" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>1604</v>
       </c>
@@ -27141,7 +27144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="356" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>1612</v>
       </c>
@@ -27200,7 +27203,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="357" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>1613</v>
       </c>
@@ -27259,7 +27262,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="358" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>1614</v>
       </c>
@@ -27318,7 +27321,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="359" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>1617</v>
       </c>
@@ -27377,7 +27380,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="360" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>1622</v>
       </c>
@@ -27424,7 +27427,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="361" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>1625</v>
       </c>
@@ -27483,7 +27486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="362" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>1627</v>
       </c>
@@ -27542,7 +27545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="363" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>1635</v>
       </c>
@@ -27601,7 +27604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="364" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>1639</v>
       </c>
@@ -27660,7 +27663,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="365" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>1644</v>
       </c>
@@ -27719,7 +27722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="366" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>1656</v>
       </c>
@@ -27778,7 +27781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="367" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>1664</v>
       </c>
@@ -27825,7 +27828,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="368" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>1669</v>
       </c>
@@ -27884,7 +27887,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="369" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>1677</v>
       </c>
@@ -27943,7 +27946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="370" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>1678</v>
       </c>
@@ -28002,7 +28005,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="371" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>1681</v>
       </c>
@@ -28061,7 +28064,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="372" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>1689</v>
       </c>
@@ -28120,7 +28123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="373" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>1692</v>
       </c>
@@ -28179,7 +28182,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="374" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>1696</v>
       </c>
@@ -28238,7 +28241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="375" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>1701</v>
       </c>
@@ -28297,7 +28300,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="376" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>1705</v>
       </c>
@@ -28356,7 +28359,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="377" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>1711</v>
       </c>
@@ -28415,7 +28418,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="378" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>1715</v>
       </c>
@@ -28474,7 +28477,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="379" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>1720</v>
       </c>
@@ -28533,7 +28536,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="380" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>1725</v>
       </c>
@@ -28592,7 +28595,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="381" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>1733</v>
       </c>
@@ -28651,7 +28654,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="382" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>1744</v>
       </c>
@@ -28710,7 +28713,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="383" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>1753</v>
       </c>
@@ -28769,7 +28772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="384" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>1756</v>
       </c>
@@ -28816,7 +28819,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="385" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>1769</v>
       </c>
@@ -28875,7 +28878,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="386" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>1775</v>
       </c>
@@ -28934,7 +28937,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="387" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>1779</v>
       </c>
@@ -28993,7 +28996,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="388" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>1788</v>
       </c>
@@ -29042,7 +29045,7 @@
       <c r="Q388" s="1"/>
       <c r="R388" s="2"/>
     </row>
-    <row r="389" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>1790</v>
       </c>
@@ -29101,7 +29104,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="390" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>1800</v>
       </c>
@@ -29160,7 +29163,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="391" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>1807</v>
       </c>
@@ -29209,7 +29212,7 @@
       <c r="Q391" s="1"/>
       <c r="R391" s="2"/>
     </row>
-    <row r="392" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>1812</v>
       </c>
@@ -29268,7 +29271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="393" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>1818</v>
       </c>
@@ -29327,7 +29330,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="394" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>1826</v>
       </c>
@@ -29386,7 +29389,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="395" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>1831</v>
       </c>
@@ -29445,7 +29448,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="396" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>1838</v>
       </c>
@@ -29507,7 +29510,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="397" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>1850</v>
       </c>
@@ -29554,7 +29557,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="398" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>1852</v>
       </c>
@@ -29601,7 +29604,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="399" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>1868</v>
       </c>
@@ -29660,7 +29663,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="400" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>1876</v>
       </c>
@@ -29719,7 +29722,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="401" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>1877</v>
       </c>
@@ -29778,7 +29781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="402" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>1878</v>
       </c>
@@ -29837,7 +29840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="403" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>1880</v>
       </c>
@@ -29896,7 +29899,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="404" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>1887</v>
       </c>
@@ -29955,7 +29958,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="405" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>1890</v>
       </c>
@@ -30002,7 +30005,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="406" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>1893</v>
       </c>
@@ -30061,7 +30064,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="407" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>1894</v>
       </c>
@@ -30120,7 +30123,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="408" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>1899</v>
       </c>
@@ -30179,7 +30182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="409" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>1915</v>
       </c>
@@ -30238,7 +30241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="410" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>1928</v>
       </c>
@@ -30297,7 +30300,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="411" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>1933</v>
       </c>
@@ -30356,7 +30359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="412" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>1935</v>
       </c>
@@ -30418,7 +30421,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="413" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>1960</v>
       </c>
@@ -30477,7 +30480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="414" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>1966</v>
       </c>
@@ -30536,67 +30539,67 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="415" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E415"/>
     </row>
-    <row r="416" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E416"/>
     </row>
-    <row r="417" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="417" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E417"/>
     </row>
-    <row r="418" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="418" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E418"/>
     </row>
-    <row r="419" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="419" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E419"/>
     </row>
-    <row r="420" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="420" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E420"/>
     </row>
-    <row r="421" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="421" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E421"/>
     </row>
-    <row r="422" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="422" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E422"/>
     </row>
-    <row r="423" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="423" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E423"/>
     </row>
-    <row r="424" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="424" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E424"/>
     </row>
-    <row r="425" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="425" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E425"/>
     </row>
-    <row r="426" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="426" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E426"/>
     </row>
-    <row r="427" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="427" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E427"/>
     </row>
-    <row r="428" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="428" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E428"/>
     </row>
-    <row r="429" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="429" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E429"/>
     </row>
-    <row r="430" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="430" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E430"/>
     </row>
-    <row r="431" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="431" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E431"/>
     </row>
-    <row r="432" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="432" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E432"/>
     </row>
-    <row r="433" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="433" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E433"/>
     </row>
-    <row r="434" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="434" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E434"/>
     </row>
-    <row r="435" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="435" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E435"/>
     </row>
   </sheetData>
@@ -30831,29 +30834,29 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="47.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.7265625" customWidth="1"/>
-    <col min="14" max="14" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -30915,7 +30918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1948</v>
       </c>
@@ -30977,7 +30980,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1949</v>
       </c>
@@ -31039,7 +31042,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -31061,7 +31064,7 @@
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>1724</v>
       </c>
@@ -31102,7 +31105,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1725</v>
       </c>
@@ -31146,7 +31149,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>1726</v>
       </c>
@@ -31187,7 +31190,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>1727</v>
       </c>
@@ -31228,7 +31231,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>1728</v>
       </c>
@@ -31269,7 +31272,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>1729</v>
       </c>
@@ -31310,7 +31313,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>1730</v>
       </c>
@@ -31351,7 +31354,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>1731</v>
       </c>
@@ -31395,7 +31398,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>1732</v>
       </c>
@@ -31439,7 +31442,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>1733</v>
       </c>
@@ -31480,7 +31483,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>1734</v>
       </c>
@@ -31521,7 +31524,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>1764</v>
       </c>
@@ -31562,7 +31565,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>1765</v>
       </c>
@@ -31603,7 +31606,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>1766</v>
       </c>
@@ -31644,7 +31647,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>1767</v>
       </c>
@@ -31685,7 +31688,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>1768</v>
       </c>
@@ -31726,7 +31729,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>1783</v>
       </c>
@@ -31767,7 +31770,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>1784</v>
       </c>
@@ -31808,7 +31811,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>1787</v>
       </c>
@@ -31852,7 +31855,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>1788</v>
       </c>
@@ -31896,12 +31899,12 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>1735</v>
       </c>
@@ -31945,7 +31948,7 @@
         <v>1742</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>1736</v>
       </c>
@@ -31989,7 +31992,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>1737</v>
       </c>
@@ -32033,7 +32036,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>1738</v>
       </c>
@@ -32077,7 +32080,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E32" s="10"/>
     </row>
   </sheetData>
@@ -32099,16 +32102,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1947</v>
       </c>
@@ -32152,7 +32155,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -32203,7 +32206,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1761</v>
       </c>
@@ -32254,7 +32257,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -32305,7 +32308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1642</v>
       </c>
@@ -32356,7 +32359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1685</v>
       </c>
@@ -32388,7 +32391,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1762</v>
       </c>
@@ -32432,7 +32435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1671</v>
       </c>
@@ -32469,7 +32472,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1741</v>
       </c>
@@ -32485,7 +32488,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -32508,14 +32511,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="D11" t="s">
         <v>1909</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>1763</v>
       </c>
@@ -32531,7 +32534,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>1655</v>
       </c>
@@ -32541,18 +32544,18 @@
       </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>1758</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1759</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1760</v>
       </c>
@@ -32576,29 +32579,29 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.7265625" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" customWidth="1"/>
-    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -32660,7 +32663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1956</v>
       </c>
@@ -32701,7 +32704,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>289</v>
       </c>
@@ -32742,7 +32745,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1695</v>
       </c>

</xml_diff>

<commit_message>
minor edit to add grey noddy proof
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3EFCEB-7B60-477A-A03A-83FE253BA7FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE6CD2B-C6AD-4792-B7F1-54F23128E3CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB - Primary List" sheetId="1" r:id="rId1"/>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7368" uniqueCount="1994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7372" uniqueCount="1998">
   <si>
     <t>Taxon Sort</t>
   </si>
@@ -6232,6 +6232,18 @@
   </si>
   <si>
     <t>New Holland x White-cheeked Honeyeater</t>
+  </si>
+  <si>
+    <t>406_Grey Ternlet_01.jpg</t>
+  </si>
+  <si>
+    <t>https://macaulaylibrary.org/asset/144434481</t>
+  </si>
+  <si>
+    <t>Moreton Bay off Wynnum</t>
+  </si>
+  <si>
+    <t>Lena Chi</t>
   </si>
 </sst>
 </file>
@@ -6808,12 +6820,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787458D5-0D53-4EB5-974E-BD980B126E90}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:V435"/>
+  <dimension ref="A1:U435"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A373" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C400" sqref="C400"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8641,7 +8652,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2127</v>
       </c>
@@ -9502,7 +9513,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3194</v>
       </c>
@@ -10050,7 +10061,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3358</v>
       </c>
@@ -12112,7 +12123,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>5706</v>
       </c>
@@ -14187,7 +14198,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>6025</v>
       </c>
@@ -14289,7 +14300,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="123" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>6075</v>
       </c>
@@ -14875,7 +14886,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="133" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>6321</v>
       </c>
@@ -14919,15 +14930,28 @@
         <v>1834</v>
       </c>
       <c r="O133" t="s">
-        <v>1814</v>
-      </c>
-      <c r="Q133" s="1"/>
-      <c r="R133" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="P133" t="s">
+        <v>1994</v>
+      </c>
+      <c r="Q133" s="1" t="s">
+        <v>1995</v>
+      </c>
+      <c r="R133" s="2">
+        <v>43533</v>
+      </c>
+      <c r="S133" t="s">
+        <v>1996</v>
+      </c>
+      <c r="T133" t="s">
+        <v>1997</v>
+      </c>
       <c r="U133">
         <v>406</v>
       </c>
     </row>
-    <row r="134" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>6331</v>
       </c>
@@ -15612,7 +15636,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="145" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>6481</v>
       </c>
@@ -15677,7 +15701,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="146" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>6492</v>
       </c>
@@ -15742,7 +15766,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="147" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>6519</v>
       </c>
@@ -15869,7 +15893,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="149" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>6544</v>
       </c>
@@ -15934,7 +15958,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="150" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>6545</v>
       </c>
@@ -15984,7 +16008,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="151" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>6546</v>
       </c>
@@ -16101,7 +16125,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="153" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>6557</v>
       </c>
@@ -16153,7 +16177,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="154" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>6561</v>
       </c>
@@ -16519,7 +16543,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="161" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>6650</v>
       </c>
@@ -16808,7 +16832,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="166" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>6677</v>
       </c>
@@ -16858,7 +16882,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="167" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>6681</v>
       </c>
@@ -16908,7 +16932,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="168" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>6682</v>
       </c>
@@ -17147,7 +17171,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="172" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>6707</v>
       </c>
@@ -17247,7 +17271,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="174" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>6716</v>
       </c>
@@ -17488,7 +17512,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="178" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>6739</v>
       </c>
@@ -17540,7 +17564,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="179" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>6741</v>
       </c>
@@ -17932,7 +17956,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="186" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>6777</v>
       </c>
@@ -18108,7 +18132,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="189" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>6855</v>
       </c>
@@ -18780,7 +18804,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="200" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>7003</v>
       </c>
@@ -19949,7 +19973,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="219" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>7313</v>
       </c>
@@ -20609,7 +20633,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="230" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>7804</v>
       </c>
@@ -23204,7 +23228,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="273" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>11798</v>
       </c>
@@ -23256,7 +23280,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="274" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>11810</v>
       </c>
@@ -24400,7 +24424,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="293" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>16890</v>
       </c>
@@ -26546,7 +26570,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="328" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>17501</v>
       </c>
@@ -30872,7 +30896,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="399" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>28322</v>
       </c>
@@ -31421,7 +31445,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="408" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>34104</v>
       </c>
@@ -31659,7 +31683,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="412" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>34133</v>
       </c>
@@ -31899,13 +31923,7 @@
       <c r="E435"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T414" xr:uid="{19B4AC61-4D89-4886-A4F3-71B43E4AFDAA}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:T414" xr:uid="{19B4AC61-4D89-4886-A4F3-71B43E4AFDAA}"/>
   <sortState ref="A2:U414">
     <sortCondition ref="U1"/>
   </sortState>
@@ -32121,10 +32139,11 @@
     <hyperlink ref="Q259" r:id="rId209" xr:uid="{B56B0650-0B6D-4FE8-B110-7AAD0678C5FE}"/>
     <hyperlink ref="Q258" r:id="rId210" xr:uid="{F0942B82-A764-49DA-A8AB-84F5AF6CB634}"/>
     <hyperlink ref="Q174" r:id="rId211" xr:uid="{B2CD6B08-E97E-41F0-A3D8-9A84E89D5B71}"/>
+    <hyperlink ref="Q133" r:id="rId212" xr:uid="{D3385EE0-5F7D-407E-B4C1-3D0032A601A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId212"/>
-  <legacyDrawing r:id="rId213"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId213"/>
+  <legacyDrawing r:id="rId214"/>
 </worksheet>
 </file>
 
@@ -32133,7 +32152,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32401,7 +32420,7 @@
         <v>1682</v>
       </c>
       <c r="L5" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M5" t="s">
         <v>1683</v>
@@ -32442,7 +32461,7 @@
         <v>1682</v>
       </c>
       <c r="L6" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M6" t="s">
         <v>1683</v>
@@ -33884,7 +33903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04E6990-0DE1-4FFF-9BE3-82E036D7135B}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new species, surveyor sheet formatting
try #118
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AD7386-CEE8-4F84-95DC-2D00BCE126EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6524DBC-CA2E-41AF-A43F-5A7D099D92DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="1" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB - Primary List" sheetId="1" r:id="rId1"/>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7413" uniqueCount="2009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7418" uniqueCount="2009">
   <si>
     <t>Taxon Sort</t>
   </si>
@@ -6267,9 +6267,6 @@
     <t>Muscovy Duck x Mallard</t>
   </si>
   <si>
-    <t>Cox's Sandpiper</t>
-  </si>
-  <si>
     <t>G00272</t>
   </si>
   <si>
@@ -6277,6 +6274,9 @@
   </si>
   <si>
     <t>Anser sp. (Domestic type)</t>
+  </si>
+  <si>
+    <t>"Cox's" Sandpiper</t>
   </si>
 </sst>
 </file>
@@ -6857,7 +6857,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12067,7 +12067,7 @@
         <v>1682</v>
       </c>
       <c r="L85" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M85" t="s">
         <v>1683</v>
@@ -14954,7 +14954,7 @@
         <v>1682</v>
       </c>
       <c r="L133" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M133" t="s">
         <v>1683</v>
@@ -15019,7 +15019,7 @@
         <v>1682</v>
       </c>
       <c r="L134" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M134" t="s">
         <v>1683</v>
@@ -15704,7 +15704,7 @@
         <v>1682</v>
       </c>
       <c r="L145" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M145" t="s">
         <v>1683</v>
@@ -15769,7 +15769,7 @@
         <v>1682</v>
       </c>
       <c r="L146" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M146" t="s">
         <v>1683</v>
@@ -15834,7 +15834,7 @@
         <v>1682</v>
       </c>
       <c r="L147" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M147" t="s">
         <v>1683</v>
@@ -15949,7 +15949,7 @@
         <v>1682</v>
       </c>
       <c r="L149" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M149" t="s">
         <v>1683</v>
@@ -16064,7 +16064,7 @@
         <v>1682</v>
       </c>
       <c r="L151" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M151" t="s">
         <v>1683</v>
@@ -16561,7 +16561,7 @@
         <v>1682</v>
       </c>
       <c r="L160" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M160" t="s">
         <v>1683</v>
@@ -16850,7 +16850,7 @@
         <v>1682</v>
       </c>
       <c r="L165" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M165" t="s">
         <v>1683</v>
@@ -17289,7 +17289,7 @@
         <v>1682</v>
       </c>
       <c r="L173" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M173" t="s">
         <v>1683</v>
@@ -18842,25 +18842,25 @@
         <v>697</v>
       </c>
       <c r="F200" t="s">
-        <v>499</v>
+        <v>1740</v>
       </c>
       <c r="G200" t="s">
         <v>20</v>
       </c>
       <c r="H200" t="s">
-        <v>499</v>
+        <v>1740</v>
       </c>
       <c r="I200" t="s">
-        <v>499</v>
+        <v>1740</v>
       </c>
       <c r="J200" t="s">
-        <v>499</v>
+        <v>1740</v>
       </c>
       <c r="K200" t="s">
         <v>1682</v>
       </c>
       <c r="L200" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M200" t="s">
         <v>1683</v>
@@ -30961,7 +30961,7 @@
         <v>1682</v>
       </c>
       <c r="L399" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M399" t="s">
         <v>1683</v>
@@ -32184,8 +32184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFAC224-3B06-46C1-8FBC-4E0275C3F461}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32538,7 +32538,7 @@
         <v>1682</v>
       </c>
       <c r="L7" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M7" t="s">
         <v>1683</v>
@@ -32620,7 +32620,7 @@
         <v>1682</v>
       </c>
       <c r="L9" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M9" t="s">
         <v>1683</v>
@@ -32743,7 +32743,7 @@
         <v>1682</v>
       </c>
       <c r="L12" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M12" t="s">
         <v>1683</v>
@@ -32872,7 +32872,7 @@
         <v>1682</v>
       </c>
       <c r="L15" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M15" t="s">
         <v>1683</v>
@@ -32913,7 +32913,7 @@
         <v>1682</v>
       </c>
       <c r="L16" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M16" t="s">
         <v>1683</v>
@@ -32995,7 +32995,7 @@
         <v>1682</v>
       </c>
       <c r="L19" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M19" t="s">
         <v>1683</v>
@@ -33003,19 +33003,19 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>1720</v>
       </c>
       <c r="C20" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2006</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>2007</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2007</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>2008</v>
       </c>
       <c r="F20" t="s">
         <v>1748</v>
@@ -33036,7 +33036,7 @@
         <v>1682</v>
       </c>
       <c r="L20" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M20" t="s">
         <v>1683</v>
@@ -33326,7 +33326,7 @@
         <v>1682</v>
       </c>
       <c r="L27" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M27" t="s">
         <v>1683</v>
@@ -33375,7 +33375,7 @@
         <v>1682</v>
       </c>
       <c r="L29" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M29" t="s">
         <v>1683</v>
@@ -33419,7 +33419,7 @@
         <v>1682</v>
       </c>
       <c r="L30" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M30" t="s">
         <v>1683</v>
@@ -33439,7 +33439,7 @@
         <v>1727</v>
       </c>
       <c r="D31" t="s">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>1729</v>
@@ -33463,7 +33463,7 @@
         <v>1682</v>
       </c>
       <c r="L31" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M31" t="s">
         <v>1683</v>
@@ -33507,7 +33507,7 @@
         <v>1682</v>
       </c>
       <c r="L32" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M32" t="s">
         <v>1683</v>
@@ -33551,7 +33551,7 @@
         <v>1682</v>
       </c>
       <c r="L33" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="M33" t="s">
         <v>1683</v>
@@ -33586,7 +33586,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33778,7 +33778,7 @@
       </c>
       <c r="N4" s="15">
         <f t="shared" ca="1" si="4"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>1665</v>
@@ -33829,7 +33829,7 @@
       </c>
       <c r="N5" s="16">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P5" s="16" t="s">
         <v>1657</v>
@@ -33843,7 +33843,7 @@
       </c>
       <c r="T5" s="16">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -33882,7 +33882,7 @@
       </c>
       <c r="T6" s="15">
         <f t="shared" ref="T6" ca="1" si="6">SUMPRODUCT(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!F:F"),S6))</f>
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33905,7 +33905,7 @@
       </c>
       <c r="K7" s="16">
         <f t="shared" ca="1" si="1"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>1906</v>
@@ -33949,7 +33949,7 @@
       </c>
       <c r="K8" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P8" s="15" t="s">
         <v>1661</v>
@@ -33979,7 +33979,7 @@
       </c>
       <c r="Q9" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -34002,7 +34002,7 @@
       </c>
       <c r="Q10" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -34020,6 +34020,12 @@
         <f ca="1">B2+B4+B10</f>
         <v>413</v>
       </c>
+      <c r="D12" s="11" t="s">
+        <v>1937</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>1655</v>
+      </c>
       <c r="P12" s="11" t="s">
         <v>1906</v>
       </c>
@@ -34037,19 +34043,41 @@
         <v>442</v>
       </c>
       <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D13" s="14" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E13" s="15">
+        <f ca="1">SUM(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!L:L"),D13), COUNTIF(INDIRECT("'"&amp;$A$17:$A$17&amp;"'!L:L"),D13))</f>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="16" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E14" s="16">
+        <f ca="1">SUM(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!L:L"),D14), COUNTIF(INDIRECT("'"&amp;$A$17:$A$17&amp;"'!L:L"),D14))</f>
+        <v>23</v>
+      </c>
+    </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>1742</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1743</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D16" s="11" t="s">
+        <v>1906</v>
+      </c>
+      <c r="E16" s="12">
+        <f ca="1">SUM(E13:E14)</f>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1744</v>
       </c>
@@ -34069,7 +34097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04E6990-0DE1-4FFF-9BE3-82E036D7135B}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish crested pigeon draft
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD06324A-D661-40F9-BEF2-E1219500F163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5C50EF-6BF2-44A0-A508-5671038F153D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB - Primary List" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ABB - Primary List'!$A$1:$T$413</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ABB - Supplementary Lists'!$A$1:$T$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Quick Tables'!$G$1:$H$5</definedName>
-    <definedName name="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R181" hidden="1">'ABB - Primary List'!$B$261:$N$261</definedName>
+    <definedName name="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R18" hidden="1">'ABB - Primary List'!$B$261:$N$261</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,6 +39,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -241,7 +242,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range 1" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R181"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_ABBSupplementaryListsA1R18"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -6856,39 +6857,39 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U434"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M132" sqref="M132"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.1796875" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.26953125" customWidth="1"/>
+    <col min="22" max="22" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6953,7 +6954,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>215</v>
       </c>
@@ -7018,7 +7019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>217</v>
       </c>
@@ -7083,7 +7084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>227</v>
       </c>
@@ -7148,7 +7149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>326</v>
       </c>
@@ -7210,7 +7211,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>329</v>
       </c>
@@ -7272,7 +7273,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>360</v>
       </c>
@@ -7334,7 +7335,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>387</v>
       </c>
@@ -7396,7 +7397,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>395</v>
       </c>
@@ -7458,7 +7459,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>426</v>
       </c>
@@ -7520,7 +7521,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>452</v>
       </c>
@@ -7582,7 +7583,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>539</v>
       </c>
@@ -7644,7 +7645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>543</v>
       </c>
@@ -7706,7 +7707,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>554</v>
       </c>
@@ -7768,7 +7769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>578</v>
       </c>
@@ -7830,7 +7831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>673</v>
       </c>
@@ -7892,7 +7893,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>678</v>
       </c>
@@ -7954,7 +7955,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1162</v>
       </c>
@@ -8016,7 +8017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1173</v>
       </c>
@@ -8078,7 +8079,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1193</v>
       </c>
@@ -8128,7 +8129,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1727</v>
       </c>
@@ -8190,7 +8191,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1747</v>
       </c>
@@ -8252,7 +8253,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1759</v>
       </c>
@@ -8314,7 +8315,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1799</v>
       </c>
@@ -8376,7 +8377,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1867</v>
       </c>
@@ -8438,7 +8439,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1986</v>
       </c>
@@ -8500,7 +8501,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2002</v>
       </c>
@@ -8562,7 +8563,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2089</v>
       </c>
@@ -8624,7 +8625,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2126</v>
       </c>
@@ -8686,7 +8687,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2131</v>
       </c>
@@ -8724,7 +8725,7 @@
         <v>1681</v>
       </c>
       <c r="M30" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="O30" t="s">
         <v>23</v>
@@ -8748,7 +8749,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2149</v>
       </c>
@@ -8810,7 +8811,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2150</v>
       </c>
@@ -8875,7 +8876,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2152</v>
       </c>
@@ -8937,7 +8938,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2157</v>
       </c>
@@ -8999,7 +9000,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2517</v>
       </c>
@@ -9061,7 +9062,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2536</v>
       </c>
@@ -9123,7 +9124,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2552</v>
       </c>
@@ -9185,7 +9186,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2743</v>
       </c>
@@ -9247,7 +9248,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>3039</v>
       </c>
@@ -9309,7 +9310,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>3162</v>
       </c>
@@ -9371,7 +9372,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>3173</v>
       </c>
@@ -9433,7 +9434,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>3193</v>
       </c>
@@ -9495,7 +9496,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>3194</v>
       </c>
@@ -9547,7 +9548,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>3196</v>
       </c>
@@ -9609,7 +9610,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>3202</v>
       </c>
@@ -9671,7 +9672,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3222</v>
       </c>
@@ -9733,7 +9734,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>3228</v>
       </c>
@@ -9795,7 +9796,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>3250</v>
       </c>
@@ -9857,7 +9858,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>3317</v>
       </c>
@@ -9919,7 +9920,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3323</v>
       </c>
@@ -9981,7 +9982,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>3327</v>
       </c>
@@ -10043,7 +10044,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>3358</v>
       </c>
@@ -10095,7 +10096,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>3361</v>
       </c>
@@ -10157,7 +10158,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>3677</v>
       </c>
@@ -10219,7 +10220,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>3779</v>
       </c>
@@ -10281,7 +10282,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>3864</v>
       </c>
@@ -10328,7 +10329,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>3984</v>
       </c>
@@ -10390,7 +10391,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>5121</v>
       </c>
@@ -10452,7 +10453,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>5150</v>
       </c>
@@ -10514,7 +10515,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>5228</v>
       </c>
@@ -10564,7 +10565,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>5236</v>
       </c>
@@ -10626,7 +10627,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>5258</v>
       </c>
@@ -10688,7 +10689,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5268</v>
       </c>
@@ -10750,7 +10751,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>5298</v>
       </c>
@@ -10812,7 +10813,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>5328</v>
       </c>
@@ -10874,7 +10875,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>5372</v>
       </c>
@@ -10936,7 +10937,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>5387</v>
       </c>
@@ -10998,7 +10999,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>5487</v>
       </c>
@@ -11060,7 +11061,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>5527</v>
       </c>
@@ -11122,7 +11123,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>5530</v>
       </c>
@@ -11184,7 +11185,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>5533</v>
       </c>
@@ -11246,7 +11247,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>5546</v>
       </c>
@@ -11308,7 +11309,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>5557</v>
       </c>
@@ -11370,7 +11371,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>5558</v>
       </c>
@@ -11432,7 +11433,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>5562</v>
       </c>
@@ -11497,7 +11498,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>5576</v>
       </c>
@@ -11559,7 +11560,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>5581</v>
       </c>
@@ -11621,7 +11622,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>5621</v>
       </c>
@@ -11671,7 +11672,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>5622</v>
       </c>
@@ -11733,7 +11734,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>5639</v>
       </c>
@@ -11795,7 +11796,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>5647</v>
       </c>
@@ -11857,7 +11858,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>5656</v>
       </c>
@@ -11919,7 +11920,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>5660</v>
       </c>
@@ -11981,7 +11982,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>5706</v>
       </c>
@@ -12046,7 +12047,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>5711</v>
       </c>
@@ -12108,7 +12109,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>5714</v>
       </c>
@@ -12170,7 +12171,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>5734</v>
       </c>
@@ -12232,7 +12233,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>5739</v>
       </c>
@@ -12294,7 +12295,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>5762</v>
       </c>
@@ -12356,7 +12357,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>5768</v>
       </c>
@@ -12406,7 +12407,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>5773</v>
       </c>
@@ -12468,7 +12469,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>5781</v>
       </c>
@@ -12530,7 +12531,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>5786</v>
       </c>
@@ -12592,7 +12593,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>5795</v>
       </c>
@@ -12654,7 +12655,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>5803</v>
       </c>
@@ -12716,7 +12717,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>5804</v>
       </c>
@@ -12778,7 +12779,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>5814</v>
       </c>
@@ -12840,7 +12841,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>5815</v>
       </c>
@@ -12902,7 +12903,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>5818</v>
       </c>
@@ -12964,7 +12965,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>5820</v>
       </c>
@@ -13026,7 +13027,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>5822</v>
       </c>
@@ -13088,7 +13089,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>5824</v>
       </c>
@@ -13150,7 +13151,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>5825</v>
       </c>
@@ -13212,7 +13213,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>5854</v>
       </c>
@@ -13274,7 +13275,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>5856</v>
       </c>
@@ -13336,7 +13337,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>5864</v>
       </c>
@@ -13398,7 +13399,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>5895</v>
       </c>
@@ -13460,7 +13461,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>5923</v>
       </c>
@@ -13522,7 +13523,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>5929</v>
       </c>
@@ -13584,7 +13585,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>5936</v>
       </c>
@@ -13646,7 +13647,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>5937</v>
       </c>
@@ -13696,7 +13697,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>5941</v>
       </c>
@@ -13758,7 +13759,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>5947</v>
       </c>
@@ -13808,7 +13809,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>5949</v>
       </c>
@@ -13870,7 +13871,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>5950</v>
       </c>
@@ -13932,7 +13933,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>5971</v>
       </c>
@@ -13994,7 +13995,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>6014</v>
       </c>
@@ -14056,7 +14057,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>6017</v>
       </c>
@@ -14118,7 +14119,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>6024</v>
       </c>
@@ -14180,7 +14181,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="120" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>6025</v>
       </c>
@@ -14232,7 +14233,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>6055</v>
       </c>
@@ -14282,7 +14283,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="122" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>6075</v>
       </c>
@@ -14334,7 +14335,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>6080</v>
       </c>
@@ -14396,7 +14397,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>6081</v>
       </c>
@@ -14458,7 +14459,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>6083</v>
       </c>
@@ -14508,7 +14509,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>6178</v>
       </c>
@@ -14570,7 +14571,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>6198</v>
       </c>
@@ -14632,7 +14633,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>6213</v>
       </c>
@@ -14682,7 +14683,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>6292</v>
       </c>
@@ -14744,7 +14745,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>6301</v>
       </c>
@@ -14806,7 +14807,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>6307</v>
       </c>
@@ -14868,7 +14869,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>6321</v>
       </c>
@@ -14933,7 +14934,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>6331</v>
       </c>
@@ -14998,7 +14999,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>6337</v>
       </c>
@@ -15060,7 +15061,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>6347</v>
       </c>
@@ -15122,7 +15123,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>6356</v>
       </c>
@@ -15184,7 +15185,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>6383</v>
       </c>
@@ -15246,7 +15247,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>6391</v>
       </c>
@@ -15308,7 +15309,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>6396</v>
       </c>
@@ -15370,7 +15371,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>6397</v>
       </c>
@@ -15432,7 +15433,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>6416</v>
       </c>
@@ -15494,7 +15495,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>6447</v>
       </c>
@@ -15556,7 +15557,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>6460</v>
       </c>
@@ -15618,7 +15619,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>6481</v>
       </c>
@@ -15683,7 +15684,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>6492</v>
       </c>
@@ -15748,7 +15749,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>6519</v>
       </c>
@@ -15813,7 +15814,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>6541</v>
       </c>
@@ -15863,7 +15864,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>6544</v>
       </c>
@@ -15928,7 +15929,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="149" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>6545</v>
       </c>
@@ -15978,7 +15979,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>6546</v>
       </c>
@@ -16043,7 +16044,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>6552</v>
       </c>
@@ -16093,7 +16094,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="152" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>6557</v>
       </c>
@@ -16145,7 +16146,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="153" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>6561</v>
       </c>
@@ -16197,7 +16198,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>6574</v>
       </c>
@@ -16259,7 +16260,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>6585</v>
       </c>
@@ -16311,7 +16312,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>6592</v>
       </c>
@@ -16363,7 +16364,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>6600</v>
       </c>
@@ -16425,7 +16426,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>6643</v>
       </c>
@@ -16475,7 +16476,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>6650</v>
       </c>
@@ -16540,7 +16541,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>6652</v>
       </c>
@@ -16590,7 +16591,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>6660</v>
       </c>
@@ -16652,7 +16653,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>6662</v>
       </c>
@@ -16702,7 +16703,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>6670</v>
       </c>
@@ -16764,7 +16765,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>6682</v>
       </c>
@@ -16829,7 +16830,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="165" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>6677</v>
       </c>
@@ -16879,7 +16880,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="166" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>6681</v>
       </c>
@@ -16929,7 +16930,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>6695</v>
       </c>
@@ -16979,7 +16980,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>6699</v>
       </c>
@@ -17041,7 +17042,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>6701</v>
       </c>
@@ -17091,7 +17092,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>6714</v>
       </c>
@@ -17153,7 +17154,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="171" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>6707</v>
       </c>
@@ -17203,7 +17204,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>6716</v>
       </c>
@@ -17268,7 +17269,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>6720</v>
       </c>
@@ -17330,7 +17331,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>6724</v>
       </c>
@@ -17380,7 +17381,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>6734</v>
       </c>
@@ -17442,7 +17443,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>6744</v>
       </c>
@@ -17494,7 +17495,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="177" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>6739</v>
       </c>
@@ -17546,7 +17547,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="178" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>6741</v>
       </c>
@@ -17598,7 +17599,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>6751</v>
       </c>
@@ -17650,7 +17651,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>6754</v>
       </c>
@@ -17712,7 +17713,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>6755</v>
       </c>
@@ -17764,7 +17765,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>6757</v>
       </c>
@@ -17826,7 +17827,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>6767</v>
       </c>
@@ -17888,7 +17889,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>6775</v>
       </c>
@@ -17938,7 +17939,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="185" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>6777</v>
       </c>
@@ -17990,7 +17991,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>6832</v>
       </c>
@@ -18052,7 +18053,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>6847</v>
       </c>
@@ -18114,7 +18115,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="188" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>6855</v>
       </c>
@@ -18166,7 +18167,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>6862</v>
       </c>
@@ -18216,7 +18217,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>6873</v>
       </c>
@@ -18278,7 +18279,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>6879</v>
       </c>
@@ -18340,7 +18341,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>6887</v>
       </c>
@@ -18402,7 +18403,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>6896</v>
       </c>
@@ -18464,7 +18465,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>6897</v>
       </c>
@@ -18526,7 +18527,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>6914</v>
       </c>
@@ -18588,7 +18589,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>6934</v>
       </c>
@@ -18650,7 +18651,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>6935</v>
       </c>
@@ -18712,7 +18713,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>6986</v>
       </c>
@@ -18774,7 +18775,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>7003</v>
       </c>
@@ -18839,7 +18840,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>7010</v>
       </c>
@@ -18901,7 +18902,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>7016</v>
       </c>
@@ -18963,7 +18964,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>7056</v>
       </c>
@@ -19025,7 +19026,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>7071</v>
       </c>
@@ -19087,7 +19088,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>7077</v>
       </c>
@@ -19149,7 +19150,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>7083</v>
       </c>
@@ -19211,7 +19212,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>7087</v>
       </c>
@@ -19273,7 +19274,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>7096</v>
       </c>
@@ -19335,7 +19336,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>7117</v>
       </c>
@@ -19397,7 +19398,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>7136</v>
       </c>
@@ -19459,7 +19460,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>7176</v>
       </c>
@@ -19521,7 +19522,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>7211</v>
       </c>
@@ -19583,7 +19584,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>7240</v>
       </c>
@@ -19645,7 +19646,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>7243</v>
       </c>
@@ -19707,7 +19708,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>7267</v>
       </c>
@@ -19769,7 +19770,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>7271</v>
       </c>
@@ -19831,7 +19832,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>7294</v>
       </c>
@@ -19893,7 +19894,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>7309</v>
       </c>
@@ -19955,7 +19956,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="218" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>7313</v>
       </c>
@@ -20007,7 +20008,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>7353</v>
       </c>
@@ -20057,7 +20058,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>7356</v>
       </c>
@@ -20119,7 +20120,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>7368</v>
       </c>
@@ -20181,7 +20182,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>7513</v>
       </c>
@@ -20243,7 +20244,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>7533</v>
       </c>
@@ -20305,7 +20306,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>7587</v>
       </c>
@@ -20367,7 +20368,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>7592</v>
       </c>
@@ -20429,7 +20430,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>7676</v>
       </c>
@@ -20491,7 +20492,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>7677</v>
       </c>
@@ -20553,7 +20554,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>7736</v>
       </c>
@@ -20615,7 +20616,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="229" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>7804</v>
       </c>
@@ -20667,7 +20668,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>7810</v>
       </c>
@@ -20729,7 +20730,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>7822</v>
       </c>
@@ -20791,7 +20792,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>7823</v>
       </c>
@@ -20853,7 +20854,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>7835</v>
       </c>
@@ -20915,7 +20916,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>8021</v>
       </c>
@@ -20977,7 +20978,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>8026</v>
       </c>
@@ -21039,7 +21040,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>8044</v>
       </c>
@@ -21101,7 +21102,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>8052</v>
       </c>
@@ -21163,7 +21164,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>8729</v>
       </c>
@@ -21225,7 +21226,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>8730</v>
       </c>
@@ -21287,7 +21288,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>8737</v>
       </c>
@@ -21349,7 +21350,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>9277</v>
       </c>
@@ -21411,7 +21412,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="242" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>9360</v>
       </c>
@@ -21473,7 +21474,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>9363</v>
       </c>
@@ -21523,7 +21524,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>9460</v>
       </c>
@@ -21585,7 +21586,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>9461</v>
       </c>
@@ -21647,7 +21648,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>9513</v>
       </c>
@@ -21709,7 +21710,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>9517</v>
       </c>
@@ -21771,7 +21772,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>9715</v>
       </c>
@@ -21833,7 +21834,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>9755</v>
       </c>
@@ -21895,7 +21896,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>11330</v>
       </c>
@@ -21957,7 +21958,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>11387</v>
       </c>
@@ -22019,7 +22020,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="252" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>11391</v>
       </c>
@@ -22081,7 +22082,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="253" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>11396</v>
       </c>
@@ -22143,7 +22144,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>11417</v>
       </c>
@@ -22205,7 +22206,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="255" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>11457</v>
       </c>
@@ -22255,7 +22256,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="256" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>11463</v>
       </c>
@@ -22317,7 +22318,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>11467</v>
       </c>
@@ -22379,7 +22380,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>11475</v>
       </c>
@@ -22444,7 +22445,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>11478</v>
       </c>
@@ -22506,7 +22507,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="260" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>11482</v>
       </c>
@@ -22571,7 +22572,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>11486</v>
       </c>
@@ -22633,7 +22634,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="262" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>11502</v>
       </c>
@@ -22695,7 +22696,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="263" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>11512</v>
       </c>
@@ -22747,7 +22748,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="264" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>11557</v>
       </c>
@@ -22809,7 +22810,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>11574</v>
       </c>
@@ -22859,7 +22860,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>11730</v>
       </c>
@@ -22921,7 +22922,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>11733</v>
       </c>
@@ -22971,7 +22972,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>11762</v>
       </c>
@@ -23033,7 +23034,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>11773</v>
       </c>
@@ -23083,7 +23084,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>11779</v>
       </c>
@@ -23145,7 +23146,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>11792</v>
       </c>
@@ -23210,7 +23211,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="272" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>11798</v>
       </c>
@@ -23262,7 +23263,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="273" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>11810</v>
       </c>
@@ -23314,7 +23315,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>11909</v>
       </c>
@@ -23376,7 +23377,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="275" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>11910</v>
       </c>
@@ -23438,7 +23439,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>11934</v>
       </c>
@@ -23500,7 +23501,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="277" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>11965</v>
       </c>
@@ -23562,7 +23563,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>12631</v>
       </c>
@@ -23624,7 +23625,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>16636</v>
       </c>
@@ -23686,7 +23687,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>16656</v>
       </c>
@@ -23748,7 +23749,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>16657</v>
       </c>
@@ -23810,7 +23811,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="282" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>16676</v>
       </c>
@@ -23872,7 +23873,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>16686</v>
       </c>
@@ -23934,7 +23935,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>16687</v>
       </c>
@@ -23984,7 +23985,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>16754</v>
       </c>
@@ -24046,7 +24047,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>16762</v>
       </c>
@@ -24108,7 +24109,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>16774</v>
       </c>
@@ -24170,7 +24171,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>16793</v>
       </c>
@@ -24232,7 +24233,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>16828</v>
       </c>
@@ -24294,7 +24295,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>16877</v>
       </c>
@@ -24356,7 +24357,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="291" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>16878</v>
       </c>
@@ -24418,7 +24419,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="292" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>16890</v>
       </c>
@@ -24468,7 +24469,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>16898</v>
       </c>
@@ -24530,7 +24531,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>16899</v>
       </c>
@@ -24592,7 +24593,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="295" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>16945</v>
       </c>
@@ -24654,7 +24655,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="296" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>16946</v>
       </c>
@@ -24716,7 +24717,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="297" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>16951</v>
       </c>
@@ -24778,7 +24779,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="298" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>16952</v>
       </c>
@@ -24840,7 +24841,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="299" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>16965</v>
       </c>
@@ -24902,7 +24903,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>16981</v>
       </c>
@@ -24964,7 +24965,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>17041</v>
       </c>
@@ -25014,7 +25015,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>17092</v>
       </c>
@@ -25076,7 +25077,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="303" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>17168</v>
       </c>
@@ -25138,7 +25139,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="304" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>17191</v>
       </c>
@@ -25200,7 +25201,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>17197</v>
       </c>
@@ -25262,7 +25263,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>17206</v>
       </c>
@@ -25324,7 +25325,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>17212</v>
       </c>
@@ -25386,7 +25387,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="308" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>17216</v>
       </c>
@@ -25448,7 +25449,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>17218</v>
       </c>
@@ -25498,7 +25499,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>17224</v>
       </c>
@@ -25560,7 +25561,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>17261</v>
       </c>
@@ -25622,7 +25623,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>17262</v>
       </c>
@@ -25684,7 +25685,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>17264</v>
       </c>
@@ -25746,7 +25747,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>17293</v>
       </c>
@@ -25808,7 +25809,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="315" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>17308</v>
       </c>
@@ -25870,7 +25871,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="316" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>17316</v>
       </c>
@@ -25932,7 +25933,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="317" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A317">
         <v>17354</v>
       </c>
@@ -25994,7 +25995,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="318" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A318">
         <v>17358</v>
       </c>
@@ -26056,7 +26057,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A319">
         <v>17397</v>
       </c>
@@ -26118,7 +26119,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A320">
         <v>17421</v>
       </c>
@@ -26180,7 +26181,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="321" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A321">
         <v>17447</v>
       </c>
@@ -26242,7 +26243,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="322" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A322">
         <v>17458</v>
       </c>
@@ -26304,7 +26305,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="323" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A323">
         <v>17473</v>
       </c>
@@ -26366,7 +26367,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A324">
         <v>17480</v>
       </c>
@@ -26431,7 +26432,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="325" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A325">
         <v>17485</v>
       </c>
@@ -26493,7 +26494,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="326" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A326">
         <v>17491</v>
       </c>
@@ -26555,7 +26556,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="327" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A327">
         <v>17501</v>
       </c>
@@ -26607,7 +26608,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="328" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A328">
         <v>17510</v>
       </c>
@@ -26669,7 +26670,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="329" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A329">
         <v>17536</v>
       </c>
@@ -26731,7 +26732,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="330" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A330">
         <v>17555</v>
       </c>
@@ -26793,7 +26794,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="331" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A331">
         <v>17559</v>
       </c>
@@ -26855,7 +26856,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="332" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A332">
         <v>17583</v>
       </c>
@@ -26917,7 +26918,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="333" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A333">
         <v>17599</v>
       </c>
@@ -26979,7 +26980,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A334">
         <v>17680</v>
       </c>
@@ -27041,7 +27042,7 @@
         <v>1543</v>
       </c>
     </row>
-    <row r="335" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A335">
         <v>17692</v>
       </c>
@@ -27103,7 +27104,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="336" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A336">
         <v>18088</v>
       </c>
@@ -27165,7 +27166,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="337" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A337">
         <v>18099</v>
       </c>
@@ -27227,7 +27228,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="338" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A338">
         <v>18100</v>
       </c>
@@ -27289,7 +27290,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="339" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A339">
         <v>18102</v>
       </c>
@@ -27351,7 +27352,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="340" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A340">
         <v>18110</v>
       </c>
@@ -27413,7 +27414,7 @@
         <v>1614</v>
       </c>
     </row>
-    <row r="341" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A341">
         <v>18113</v>
       </c>
@@ -27463,7 +27464,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="342" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A342">
         <v>18122</v>
       </c>
@@ -27525,7 +27526,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="343" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A343">
         <v>18133</v>
       </c>
@@ -27587,7 +27588,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="344" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A344">
         <v>18142</v>
       </c>
@@ -27649,7 +27650,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="345" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A345">
         <v>18156</v>
       </c>
@@ -27711,7 +27712,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="346" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A346">
         <v>18298</v>
       </c>
@@ -27761,7 +27762,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="347" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A347">
         <v>18299</v>
       </c>
@@ -27823,7 +27824,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="348" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A348">
         <v>18313</v>
       </c>
@@ -27885,7 +27886,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="349" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A349">
         <v>18322</v>
       </c>
@@ -27947,7 +27948,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="350" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A350">
         <v>18434</v>
       </c>
@@ -28009,7 +28010,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="351" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A351">
         <v>18439</v>
       </c>
@@ -28071,7 +28072,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="352" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A352">
         <v>18522</v>
       </c>
@@ -28133,7 +28134,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="353" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A353">
         <v>18571</v>
       </c>
@@ -28195,7 +28196,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="354" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A354">
         <v>18587</v>
       </c>
@@ -28257,7 +28258,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="355" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A355">
         <v>18601</v>
       </c>
@@ -28319,7 +28320,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="356" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A356">
         <v>18611</v>
       </c>
@@ -28381,7 +28382,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="357" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A357">
         <v>18751</v>
       </c>
@@ -28443,7 +28444,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="358" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A358">
         <v>18825</v>
       </c>
@@ -28505,7 +28506,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="359" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A359">
         <v>19301</v>
       </c>
@@ -28567,7 +28568,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="360" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A360">
         <v>19401</v>
       </c>
@@ -28629,7 +28630,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="361" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A361">
         <v>19515</v>
       </c>
@@ -28691,7 +28692,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="362" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A362">
         <v>19614</v>
       </c>
@@ -28753,7 +28754,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="363" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A363">
         <v>19667</v>
       </c>
@@ -28815,7 +28816,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="364" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A364">
         <v>19728</v>
       </c>
@@ -28877,7 +28878,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="365" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A365">
         <v>19920</v>
       </c>
@@ -28939,7 +28940,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="366" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A366">
         <v>19952</v>
       </c>
@@ -29001,7 +29002,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="367" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A367">
         <v>19965</v>
       </c>
@@ -29063,7 +29064,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="368" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A368">
         <v>20014</v>
       </c>
@@ -29125,7 +29126,7 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="369" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A369">
         <v>20028</v>
       </c>
@@ -29187,7 +29188,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="370" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A370">
         <v>20062</v>
       </c>
@@ -29249,7 +29250,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="371" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A371">
         <v>20064</v>
       </c>
@@ -29311,7 +29312,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="372" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A372">
         <v>20067</v>
       </c>
@@ -29373,7 +29374,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="373" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A373">
         <v>20515</v>
       </c>
@@ -29435,7 +29436,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="374" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A374">
         <v>20522</v>
       </c>
@@ -29485,7 +29486,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="375" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A375">
         <v>20550</v>
       </c>
@@ -29547,7 +29548,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="376" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A376">
         <v>20609</v>
       </c>
@@ -29609,7 +29610,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="377" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A377">
         <v>20677</v>
       </c>
@@ -29671,7 +29672,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="378" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A378">
         <v>20725</v>
       </c>
@@ -29733,7 +29734,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="379" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A379">
         <v>20737</v>
       </c>
@@ -29795,7 +29796,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="380" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A380">
         <v>20739</v>
       </c>
@@ -29857,7 +29858,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="381" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A381">
         <v>20750</v>
       </c>
@@ -29907,7 +29908,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="382" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A382">
         <v>20769</v>
       </c>
@@ -29969,7 +29970,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="383" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A383">
         <v>20772</v>
       </c>
@@ -30031,7 +30032,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="384" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A384">
         <v>21070</v>
       </c>
@@ -30081,7 +30082,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="385" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A385">
         <v>21515</v>
       </c>
@@ -30143,7 +30144,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="386" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A386">
         <v>21576</v>
       </c>
@@ -30205,7 +30206,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="387" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A387">
         <v>21577</v>
       </c>
@@ -30267,7 +30268,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="388" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A388">
         <v>21647</v>
       </c>
@@ -30317,7 +30318,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="389" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A389">
         <v>23396</v>
       </c>
@@ -30379,7 +30380,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="390" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A390">
         <v>24053</v>
       </c>
@@ -30441,7 +30442,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="391" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A391">
         <v>24058</v>
       </c>
@@ -30503,7 +30504,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="392" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A392">
         <v>24059</v>
       </c>
@@ -30565,7 +30566,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="393" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A393">
         <v>24080</v>
       </c>
@@ -30627,7 +30628,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="394" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A394">
         <v>24906</v>
       </c>
@@ -30689,7 +30690,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="395" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A395">
         <v>25487</v>
       </c>
@@ -30751,7 +30752,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="396" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A396">
         <v>27675</v>
       </c>
@@ -30813,7 +30814,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="397" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A397">
         <v>27894</v>
       </c>
@@ -30875,7 +30876,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="398" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A398">
         <v>28322</v>
       </c>
@@ -30940,7 +30941,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="399" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A399">
         <v>28432</v>
       </c>
@@ -31002,7 +31003,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="400" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A400">
         <v>28477</v>
       </c>
@@ -31064,7 +31065,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="401" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A401">
         <v>28820</v>
       </c>
@@ -31126,7 +31127,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="402" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A402">
         <v>29418</v>
       </c>
@@ -31188,7 +31189,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="403" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A403">
         <v>29437</v>
       </c>
@@ -31253,7 +31254,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="404" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A404">
         <v>29452</v>
       </c>
@@ -31315,7 +31316,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="405" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A405">
         <v>30288</v>
       </c>
@@ -31365,7 +31366,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="406" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A406">
         <v>33452</v>
       </c>
@@ -31427,7 +31428,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="407" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A407">
         <v>34104</v>
       </c>
@@ -31479,7 +31480,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="408" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A408">
         <v>34109</v>
       </c>
@@ -31541,7 +31542,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="409" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A409">
         <v>34119</v>
       </c>
@@ -31603,7 +31604,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="410" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A410">
         <v>34123</v>
       </c>
@@ -31665,7 +31666,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="411" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A411">
         <v>34133</v>
       </c>
@@ -31717,7 +31718,7 @@
         <v>1807</v>
       </c>
     </row>
-    <row r="412" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A412">
         <v>34207</v>
       </c>
@@ -31779,7 +31780,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="413" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A413">
         <v>34281</v>
       </c>
@@ -31841,67 +31842,67 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="414" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:21" x14ac:dyDescent="0.35">
       <c r="E414"/>
     </row>
-    <row r="415" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:21" x14ac:dyDescent="0.35">
       <c r="E415"/>
     </row>
-    <row r="416" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:21" x14ac:dyDescent="0.35">
       <c r="E416"/>
     </row>
-    <row r="417" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E417"/>
     </row>
-    <row r="418" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E418"/>
     </row>
-    <row r="419" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E419"/>
     </row>
-    <row r="420" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E420"/>
     </row>
-    <row r="421" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E421"/>
     </row>
-    <row r="422" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E422"/>
     </row>
-    <row r="423" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E423"/>
     </row>
-    <row r="424" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E424"/>
     </row>
-    <row r="425" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E425"/>
     </row>
-    <row r="426" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E426"/>
     </row>
-    <row r="427" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E427"/>
     </row>
-    <row r="428" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E428"/>
     </row>
-    <row r="429" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E429"/>
     </row>
-    <row r="430" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E430"/>
     </row>
-    <row r="431" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E431"/>
     </row>
-    <row r="432" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E432"/>
     </row>
-    <row r="433" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E433"/>
     </row>
-    <row r="434" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E434"/>
     </row>
   </sheetData>
@@ -31912,7 +31913,7 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:U413">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U413">
     <sortCondition ref="A1"/>
   </sortState>
   <hyperlinks>
@@ -32143,29 +32144,29 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.7265625" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -32227,7 +32228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>1961</v>
       </c>
@@ -32289,7 +32290,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1960</v>
       </c>
@@ -32351,7 +32352,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -32373,7 +32374,7 @@
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>1971</v>
       </c>
@@ -32414,7 +32415,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>1973</v>
       </c>
@@ -32458,7 +32459,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>1995</v>
       </c>
@@ -32499,7 +32500,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>1972</v>
       </c>
@@ -32540,7 +32541,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>1962</v>
       </c>
@@ -32581,7 +32582,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>1963</v>
       </c>
@@ -32622,7 +32623,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>1964</v>
       </c>
@@ -32663,7 +32664,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>1965</v>
       </c>
@@ -32704,7 +32705,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>1966</v>
       </c>
@@ -32748,7 +32749,7 @@
         <v>1813</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>1967</v>
       </c>
@@ -32792,7 +32793,7 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>1968</v>
       </c>
@@ -32833,7 +32834,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>1969</v>
       </c>
@@ -32874,7 +32875,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>1974</v>
       </c>
@@ -32915,7 +32916,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>1975</v>
       </c>
@@ -32956,7 +32957,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>2003</v>
       </c>
@@ -32997,7 +32998,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>1976</v>
       </c>
@@ -33038,7 +33039,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>1977</v>
       </c>
@@ -33079,7 +33080,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>1978</v>
       </c>
@@ -33120,7 +33121,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>1979</v>
       </c>
@@ -33161,7 +33162,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>1980</v>
       </c>
@@ -33202,7 +33203,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>1981</v>
       </c>
@@ -33246,7 +33247,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>1982</v>
       </c>
@@ -33290,12 +33291,12 @@
         <v>1813</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>1999</v>
       </c>
@@ -33339,7 +33340,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>1983</v>
       </c>
@@ -33383,7 +33384,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>1984</v>
       </c>
@@ -33427,7 +33428,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>1985</v>
       </c>
@@ -33471,7 +33472,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>1986</v>
       </c>
@@ -33515,16 +33516,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E35" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:T3" xr:uid="{C3BDEECB-DEA1-4819-8F62-78B8A91245CF}">
-    <sortState ref="A2:T3">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T3">
       <sortCondition ref="A2"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A6:N16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:N16">
     <sortCondition ref="A5"/>
   </sortState>
   <hyperlinks>
@@ -33544,16 +33545,16 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>1919</v>
       </c>
@@ -33597,7 +33598,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -33648,7 +33649,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1743</v>
       </c>
@@ -33699,7 +33700,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -33750,7 +33751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1640</v>
       </c>
@@ -33801,7 +33802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1683</v>
       </c>
@@ -33840,7 +33841,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>1744</v>
       </c>
@@ -33877,7 +33878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>1669</v>
       </c>
@@ -33921,7 +33922,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1724</v>
       </c>
@@ -33937,7 +33938,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -33960,14 +33961,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="D11" t="s">
         <v>1881</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
         <v>1745</v>
       </c>
@@ -33989,7 +33990,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
         <v>1653</v>
       </c>
@@ -34006,7 +34007,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="D14" s="16" t="s">
         <v>1682</v>
       </c>
@@ -34015,7 +34016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>1740</v>
       </c>
@@ -34027,12 +34028,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1741</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>1742</v>
       </c>
@@ -34044,7 +34045,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34064,29 +34065,29 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.7265625" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -34148,7 +34149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>27669</v>
       </c>
@@ -34189,7 +34190,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5580</v>
       </c>
@@ -34230,7 +34231,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2127</v>
       </c>
@@ -34282,7 +34283,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
add 5 new species
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C30200D-1F7F-4D31-A732-FEF4995FD7C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AD99F6-BBF0-4657-8062-D3179EA549D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
+    <workbookView xWindow="-28920" yWindow="3885" windowWidth="29040" windowHeight="15840" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB - Primary List" sheetId="1" r:id="rId1"/>
@@ -6202,9 +6202,6 @@
     <t>Long-billed x Little Corella</t>
   </si>
   <si>
-    <t>New Holland x White-cheeked Honeyeater</t>
-  </si>
-  <si>
     <t>406_Grey Ternlet_01.jpg</t>
   </si>
   <si>
@@ -6296,6 +6293,9 @@
   </si>
   <si>
     <t>Atlas of the Birds of Brisbane</t>
+  </si>
+  <si>
+    <t>"Holland-Cheeked" Honeyeater</t>
   </si>
 </sst>
 </file>
@@ -6395,7 +6395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -6462,27 +6462,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6508,7 +6493,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6888,11 +6872,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787458D5-0D53-4EB5-974E-BD980B126E90}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U435"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6987,7 +6972,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>215</v>
       </c>
@@ -7052,7 +7037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>217</v>
       </c>
@@ -7117,7 +7102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>228</v>
       </c>
@@ -7182,7 +7167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>328</v>
       </c>
@@ -7244,7 +7229,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>331</v>
       </c>
@@ -7306,7 +7291,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>362</v>
       </c>
@@ -7368,7 +7353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>392</v>
       </c>
@@ -7430,7 +7415,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>401</v>
       </c>
@@ -7492,7 +7477,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>433</v>
       </c>
@@ -7554,7 +7539,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>460</v>
       </c>
@@ -7616,7 +7601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>550</v>
       </c>
@@ -7678,7 +7663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>554</v>
       </c>
@@ -7740,7 +7725,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>565</v>
       </c>
@@ -7802,7 +7787,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>589</v>
       </c>
@@ -7864,7 +7849,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>685</v>
       </c>
@@ -7926,7 +7911,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>690</v>
       </c>
@@ -7988,7 +7973,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1174</v>
       </c>
@@ -8050,7 +8035,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1185</v>
       </c>
@@ -8112,7 +8097,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1205</v>
       </c>
@@ -8162,7 +8147,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1741</v>
       </c>
@@ -8224,7 +8209,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1761</v>
       </c>
@@ -8286,7 +8271,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1773</v>
       </c>
@@ -8348,7 +8333,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1798</v>
       </c>
@@ -8410,7 +8395,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1882</v>
       </c>
@@ -8472,7 +8457,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -8534,7 +8519,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2020</v>
       </c>
@@ -8596,7 +8581,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2103</v>
       </c>
@@ -8658,7 +8643,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2140</v>
       </c>
@@ -8720,7 +8705,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2145</v>
       </c>
@@ -8782,7 +8767,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2163</v>
       </c>
@@ -8844,7 +8829,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2164</v>
       </c>
@@ -8909,7 +8894,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2166</v>
       </c>
@@ -8971,7 +8956,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2171</v>
       </c>
@@ -9033,7 +9018,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2530</v>
       </c>
@@ -9095,7 +9080,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2549</v>
       </c>
@@ -9157,7 +9142,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2565</v>
       </c>
@@ -9219,7 +9204,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2756</v>
       </c>
@@ -9281,7 +9266,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3053</v>
       </c>
@@ -9343,7 +9328,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3177</v>
       </c>
@@ -9405,7 +9390,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3188</v>
       </c>
@@ -9467,7 +9452,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3208</v>
       </c>
@@ -9581,7 +9566,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3211</v>
       </c>
@@ -9643,7 +9628,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3217</v>
       </c>
@@ -9705,7 +9690,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3237</v>
       </c>
@@ -9767,7 +9752,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3243</v>
       </c>
@@ -9829,7 +9814,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3265</v>
       </c>
@@ -9891,7 +9876,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3332</v>
       </c>
@@ -9953,7 +9938,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3338</v>
       </c>
@@ -10015,7 +10000,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3342</v>
       </c>
@@ -10129,7 +10114,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3375</v>
       </c>
@@ -10191,7 +10176,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3691</v>
       </c>
@@ -10253,7 +10238,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3794</v>
       </c>
@@ -10315,7 +10300,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3881</v>
       </c>
@@ -10362,7 +10347,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4001</v>
       </c>
@@ -10424,7 +10409,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5150</v>
       </c>
@@ -10486,7 +10471,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5180</v>
       </c>
@@ -10548,7 +10533,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5259</v>
       </c>
@@ -10598,7 +10583,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5268</v>
       </c>
@@ -10660,7 +10645,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5290</v>
       </c>
@@ -10722,7 +10707,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5299</v>
       </c>
@@ -10784,7 +10769,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5333</v>
       </c>
@@ -10846,7 +10831,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5363</v>
       </c>
@@ -10908,7 +10893,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5407</v>
       </c>
@@ -10970,7 +10955,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>5424</v>
       </c>
@@ -11032,7 +11017,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>5524</v>
       </c>
@@ -11094,7 +11079,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5565</v>
       </c>
@@ -11156,7 +11141,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5568</v>
       </c>
@@ -11218,7 +11203,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5571</v>
       </c>
@@ -11280,7 +11265,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>5585</v>
       </c>
@@ -11342,7 +11327,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5596</v>
       </c>
@@ -11404,7 +11389,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5597</v>
       </c>
@@ -11466,7 +11451,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5601</v>
       </c>
@@ -11531,7 +11516,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5615</v>
       </c>
@@ -11593,7 +11578,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5620</v>
       </c>
@@ -11655,7 +11640,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5660</v>
       </c>
@@ -11705,7 +11690,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5661</v>
       </c>
@@ -11767,7 +11752,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5678</v>
       </c>
@@ -11829,7 +11814,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>5686</v>
       </c>
@@ -11891,7 +11876,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5695</v>
       </c>
@@ -11953,7 +11938,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5699</v>
       </c>
@@ -12015,7 +12000,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5747</v>
       </c>
@@ -12050,7 +12035,7 @@
         <v>1675</v>
       </c>
       <c r="L84" t="s">
-        <v>108</v>
+        <v>1675</v>
       </c>
       <c r="M84" t="s">
         <v>1676</v>
@@ -12059,7 +12044,7 @@
         <v>408</v>
       </c>
       <c r="O84" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="P84" t="s">
         <v>1931</v>
@@ -12080,7 +12065,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>5752</v>
       </c>
@@ -12142,7 +12127,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5755</v>
       </c>
@@ -12204,7 +12189,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>5775</v>
       </c>
@@ -12266,7 +12251,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5780</v>
       </c>
@@ -12328,7 +12313,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5803</v>
       </c>
@@ -12390,7 +12375,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5809</v>
       </c>
@@ -12440,7 +12425,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5814</v>
       </c>
@@ -12502,7 +12487,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>5822</v>
       </c>
@@ -12564,7 +12549,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5827</v>
       </c>
@@ -12626,7 +12611,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5836</v>
       </c>
@@ -12688,7 +12673,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5844</v>
       </c>
@@ -12750,7 +12735,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5845</v>
       </c>
@@ -12812,7 +12797,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>5855</v>
       </c>
@@ -12874,7 +12859,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5856</v>
       </c>
@@ -12936,7 +12921,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5859</v>
       </c>
@@ -12998,7 +12983,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5861</v>
       </c>
@@ -13060,7 +13045,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5863</v>
       </c>
@@ -13122,7 +13107,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5865</v>
       </c>
@@ -13184,7 +13169,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>5866</v>
       </c>
@@ -13246,7 +13231,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>5895</v>
       </c>
@@ -13308,7 +13293,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>5897</v>
       </c>
@@ -13370,7 +13355,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>5905</v>
       </c>
@@ -13432,7 +13417,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>5935</v>
       </c>
@@ -13494,7 +13479,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>5963</v>
       </c>
@@ -13556,7 +13541,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>5969</v>
       </c>
@@ -13618,7 +13603,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>5976</v>
       </c>
@@ -13680,7 +13665,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>5977</v>
       </c>
@@ -13730,7 +13715,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>5981</v>
       </c>
@@ -13792,7 +13777,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>5987</v>
       </c>
@@ -13842,7 +13827,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>5989</v>
       </c>
@@ -13904,7 +13889,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>5990</v>
       </c>
@@ -13966,7 +13951,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>6011</v>
       </c>
@@ -14028,7 +14013,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>6053</v>
       </c>
@@ -14090,7 +14075,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>6056</v>
       </c>
@@ -14152,7 +14137,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>6063</v>
       </c>
@@ -14266,7 +14251,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>6094</v>
       </c>
@@ -14368,7 +14353,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>6119</v>
       </c>
@@ -14430,7 +14415,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>6120</v>
       </c>
@@ -14492,7 +14477,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>6122</v>
       </c>
@@ -14542,7 +14527,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>6216</v>
       </c>
@@ -14604,7 +14589,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>6238</v>
       </c>
@@ -14666,7 +14651,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>6253</v>
       </c>
@@ -14716,7 +14701,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>6333</v>
       </c>
@@ -14778,7 +14763,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>6342</v>
       </c>
@@ -14840,7 +14825,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>6348</v>
       </c>
@@ -14902,7 +14887,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>6362</v>
       </c>
@@ -14937,7 +14922,7 @@
         <v>1675</v>
       </c>
       <c r="L132" t="s">
-        <v>108</v>
+        <v>1675</v>
       </c>
       <c r="M132" t="s">
         <v>1676</v>
@@ -14949,25 +14934,25 @@
         <v>23</v>
       </c>
       <c r="P132" t="s">
+        <v>1983</v>
+      </c>
+      <c r="Q132" s="1" t="s">
         <v>1984</v>
-      </c>
-      <c r="Q132" s="1" t="s">
-        <v>1985</v>
       </c>
       <c r="R132" s="2">
         <v>43533</v>
       </c>
       <c r="S132" t="s">
+        <v>1985</v>
+      </c>
+      <c r="T132" t="s">
         <v>1986</v>
-      </c>
-      <c r="T132" t="s">
-        <v>1987</v>
       </c>
       <c r="U132">
         <v>406</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>6372</v>
       </c>
@@ -15032,7 +15017,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>6378</v>
       </c>
@@ -15094,7 +15079,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>6388</v>
       </c>
@@ -15156,7 +15141,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>6397</v>
       </c>
@@ -15218,7 +15203,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>6424</v>
       </c>
@@ -15280,7 +15265,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>6432</v>
       </c>
@@ -15342,7 +15327,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>6437</v>
       </c>
@@ -15404,7 +15389,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>6438</v>
       </c>
@@ -15466,7 +15451,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>6457</v>
       </c>
@@ -15528,7 +15513,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>6489</v>
       </c>
@@ -15590,7 +15575,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>6502</v>
       </c>
@@ -15652,7 +15637,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>6523</v>
       </c>
@@ -15717,7 +15702,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>6534</v>
       </c>
@@ -15782,7 +15767,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>6559</v>
       </c>
@@ -15826,7 +15811,7 @@
         <v>1862</v>
       </c>
       <c r="O146" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="P146" t="s">
         <v>1934</v>
@@ -15847,7 +15832,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>6581</v>
       </c>
@@ -15897,7 +15882,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>6584</v>
       </c>
@@ -16012,7 +15997,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>6586</v>
       </c>
@@ -16077,7 +16062,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>6592</v>
       </c>
@@ -16231,7 +16216,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>6614</v>
       </c>
@@ -16293,7 +16278,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>6625</v>
       </c>
@@ -16345,7 +16330,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>6632</v>
       </c>
@@ -16397,7 +16382,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>6640</v>
       </c>
@@ -16459,7 +16444,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>6683</v>
       </c>
@@ -16509,22 +16494,22 @@
         <v>534</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>6684</v>
       </c>
       <c r="B159" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C159" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D159" t="s">
+        <v>2008</v>
+      </c>
+      <c r="E159" s="8" t="s">
         <v>2009</v>
       </c>
-      <c r="C159" t="s">
-        <v>2009</v>
-      </c>
-      <c r="D159" t="s">
-        <v>2009</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>2010</v>
-      </c>
       <c r="F159" t="s">
         <v>498</v>
       </c>
@@ -16544,7 +16529,7 @@
         <v>1675</v>
       </c>
       <c r="L159" t="s">
-        <v>108</v>
+        <v>1675</v>
       </c>
       <c r="M159" t="s">
         <v>1676</v>
@@ -16553,25 +16538,25 @@
         <v>23</v>
       </c>
       <c r="P159" t="s">
+        <v>2010</v>
+      </c>
+      <c r="Q159" s="1" t="s">
         <v>2011</v>
-      </c>
-      <c r="Q159" s="1" t="s">
-        <v>2012</v>
       </c>
       <c r="R159" s="2">
         <v>43635</v>
       </c>
       <c r="S159" t="s">
+        <v>2012</v>
+      </c>
+      <c r="T159" t="s">
         <v>2013</v>
-      </c>
-      <c r="T159" t="s">
-        <v>2014</v>
       </c>
       <c r="U159">
         <v>533</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>6691</v>
       </c>
@@ -16636,7 +16621,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>6693</v>
       </c>
@@ -16686,7 +16671,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>6702</v>
       </c>
@@ -16748,7 +16733,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>6704</v>
       </c>
@@ -16798,7 +16783,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>6712</v>
       </c>
@@ -16860,7 +16845,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>6724</v>
       </c>
@@ -17025,7 +17010,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>6737</v>
       </c>
@@ -17075,7 +17060,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>6742</v>
       </c>
@@ -17137,7 +17122,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>6744</v>
       </c>
@@ -17187,7 +17172,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>6757</v>
       </c>
@@ -17299,7 +17284,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>6759</v>
       </c>
@@ -17334,7 +17319,7 @@
         <v>1675</v>
       </c>
       <c r="L173" t="s">
-        <v>108</v>
+        <v>1675</v>
       </c>
       <c r="M173" t="s">
         <v>1676</v>
@@ -17364,7 +17349,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>6763</v>
       </c>
@@ -17426,7 +17411,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>6767</v>
       </c>
@@ -17476,7 +17461,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>6778</v>
       </c>
@@ -17538,7 +17523,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>6789</v>
       </c>
@@ -17694,7 +17679,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>6796</v>
       </c>
@@ -17746,7 +17731,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>6799</v>
       </c>
@@ -17808,7 +17793,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>6800</v>
       </c>
@@ -17860,7 +17845,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>6802</v>
       </c>
@@ -17922,7 +17907,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>6812</v>
       </c>
@@ -17984,7 +17969,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>6821</v>
       </c>
@@ -18086,7 +18071,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>6881</v>
       </c>
@@ -18148,7 +18133,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>6897</v>
       </c>
@@ -18262,7 +18247,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>6912</v>
       </c>
@@ -18312,7 +18297,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>6923</v>
       </c>
@@ -18374,7 +18359,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>6930</v>
       </c>
@@ -18436,7 +18421,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>6938</v>
       </c>
@@ -18498,7 +18483,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>6947</v>
       </c>
@@ -18560,7 +18545,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>6948</v>
       </c>
@@ -18622,7 +18607,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>6965</v>
       </c>
@@ -18684,7 +18669,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>6985</v>
       </c>
@@ -18746,7 +18731,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>6986</v>
       </c>
@@ -18808,7 +18793,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>7039</v>
       </c>
@@ -18870,7 +18855,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>7056</v>
       </c>
@@ -18935,7 +18920,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>7063</v>
       </c>
@@ -18997,7 +18982,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>7069</v>
       </c>
@@ -19059,7 +19044,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>7109</v>
       </c>
@@ -19121,7 +19106,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>7124</v>
       </c>
@@ -19183,7 +19168,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>7130</v>
       </c>
@@ -19245,7 +19230,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>7136</v>
       </c>
@@ -19307,7 +19292,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>7140</v>
       </c>
@@ -19369,7 +19354,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>7149</v>
       </c>
@@ -19431,7 +19416,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>7170</v>
       </c>
@@ -19493,7 +19478,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>7189</v>
       </c>
@@ -19555,7 +19540,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>7232</v>
       </c>
@@ -19617,7 +19602,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>7268</v>
       </c>
@@ -19679,7 +19664,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>7297</v>
       </c>
@@ -19741,7 +19726,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>7300</v>
       </c>
@@ -19803,7 +19788,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>7324</v>
       </c>
@@ -19865,7 +19850,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>7328</v>
       </c>
@@ -19927,7 +19912,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>7351</v>
       </c>
@@ -19989,7 +19974,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>7366</v>
       </c>
@@ -20103,7 +20088,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>7411</v>
       </c>
@@ -20153,7 +20138,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>7414</v>
       </c>
@@ -20215,7 +20200,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>7426</v>
       </c>
@@ -20277,7 +20262,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>7571</v>
       </c>
@@ -20339,7 +20324,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>7591</v>
       </c>
@@ -20401,7 +20386,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>7645</v>
       </c>
@@ -20463,7 +20448,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>7649</v>
       </c>
@@ -20525,7 +20510,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>7733</v>
       </c>
@@ -20587,7 +20572,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>7734</v>
       </c>
@@ -20649,7 +20634,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>7793</v>
       </c>
@@ -20763,7 +20748,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>7867</v>
       </c>
@@ -20825,7 +20810,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>7879</v>
       </c>
@@ -20887,7 +20872,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>7880</v>
       </c>
@@ -20949,7 +20934,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>7892</v>
       </c>
@@ -21011,7 +20996,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>8079</v>
       </c>
@@ -21073,7 +21058,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>8084</v>
       </c>
@@ -21135,7 +21120,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>8102</v>
       </c>
@@ -21197,7 +21182,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>8110</v>
       </c>
@@ -21259,7 +21244,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>8794</v>
       </c>
@@ -21321,7 +21306,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>8795</v>
       </c>
@@ -21383,7 +21368,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>8802</v>
       </c>
@@ -21397,7 +21382,7 @@
         <v>907</v>
       </c>
       <c r="E241" s="8" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="F241" t="s">
         <v>19</v>
@@ -21445,7 +21430,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="242" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>9339</v>
       </c>
@@ -21507,7 +21492,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>9423</v>
       </c>
@@ -21569,7 +21554,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>9426</v>
       </c>
@@ -21619,7 +21604,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>9521</v>
       </c>
@@ -21681,7 +21666,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>9522</v>
       </c>
@@ -21743,7 +21728,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>9574</v>
       </c>
@@ -21805,7 +21790,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>9578</v>
       </c>
@@ -21867,7 +21852,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>9776</v>
       </c>
@@ -21929,7 +21914,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>9816</v>
       </c>
@@ -21991,7 +21976,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>11400</v>
       </c>
@@ -22053,7 +22038,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="252" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>11457</v>
       </c>
@@ -22115,7 +22100,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="253" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>11461</v>
       </c>
@@ -22177,7 +22162,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>11466</v>
       </c>
@@ -22239,7 +22224,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="255" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>11487</v>
       </c>
@@ -22301,7 +22286,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="256" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>11527</v>
       </c>
@@ -22351,7 +22336,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>11533</v>
       </c>
@@ -22413,7 +22398,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>11537</v>
       </c>
@@ -22475,7 +22460,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>11545</v>
       </c>
@@ -22540,7 +22525,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="260" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>11548</v>
       </c>
@@ -22602,7 +22587,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>11552</v>
       </c>
@@ -22667,7 +22652,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="262" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>11556</v>
       </c>
@@ -22729,7 +22714,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="263" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>11573</v>
       </c>
@@ -22791,7 +22776,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="264" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>11583</v>
       </c>
@@ -22843,7 +22828,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>11629</v>
       </c>
@@ -22905,7 +22890,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>11646</v>
       </c>
@@ -22955,7 +22940,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>11811</v>
       </c>
@@ -23017,7 +23002,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>11814</v>
       </c>
@@ -23067,7 +23052,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>11843</v>
       </c>
@@ -23129,7 +23114,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>11854</v>
       </c>
@@ -23179,7 +23164,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>11860</v>
       </c>
@@ -23241,7 +23226,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>11874</v>
       </c>
@@ -23371,8 +23356,8 @@
       <c r="D274" t="s">
         <v>1938</v>
       </c>
-      <c r="E274" s="19" t="s">
-        <v>2008</v>
+      <c r="E274" s="8" t="s">
+        <v>2007</v>
       </c>
       <c r="F274" t="s">
         <v>1732</v>
@@ -23410,7 +23395,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="275" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>11992</v>
       </c>
@@ -23472,7 +23457,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>11993</v>
       </c>
@@ -23534,7 +23519,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="277" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>12040</v>
       </c>
@@ -23548,7 +23533,7 @@
         <v>1055</v>
       </c>
       <c r="E277" s="8" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="F277" t="s">
         <v>19</v>
@@ -23596,7 +23581,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>12053</v>
       </c>
@@ -23658,7 +23643,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>12726</v>
       </c>
@@ -23720,7 +23705,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>16743</v>
       </c>
@@ -23782,7 +23767,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>16762</v>
       </c>
@@ -23844,7 +23829,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="282" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>16763</v>
       </c>
@@ -23906,7 +23891,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>16783</v>
       </c>
@@ -23968,7 +23953,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>16793</v>
       </c>
@@ -24030,7 +24015,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>16794</v>
       </c>
@@ -24080,7 +24065,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>16861</v>
       </c>
@@ -24142,7 +24127,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>16869</v>
       </c>
@@ -24204,7 +24189,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>16881</v>
       </c>
@@ -24266,7 +24251,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>16900</v>
       </c>
@@ -24328,7 +24313,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>16935</v>
       </c>
@@ -24390,7 +24375,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="291" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>16983</v>
       </c>
@@ -24452,7 +24437,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>16984</v>
       </c>
@@ -24564,7 +24549,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>17004</v>
       </c>
@@ -24626,7 +24611,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="295" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>17005</v>
       </c>
@@ -24688,7 +24673,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="296" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>17051</v>
       </c>
@@ -24750,7 +24735,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="297" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>17052</v>
       </c>
@@ -24812,7 +24797,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="298" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>17057</v>
       </c>
@@ -24874,7 +24859,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="299" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>17058</v>
       </c>
@@ -24936,7 +24921,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>17071</v>
       </c>
@@ -24998,7 +24983,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>17087</v>
       </c>
@@ -25060,7 +25045,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>17147</v>
       </c>
@@ -25110,7 +25095,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="303" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>17198</v>
       </c>
@@ -25172,7 +25157,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="304" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>17274</v>
       </c>
@@ -25234,7 +25219,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>17297</v>
       </c>
@@ -25296,7 +25281,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>17303</v>
       </c>
@@ -25358,7 +25343,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>17312</v>
       </c>
@@ -25420,7 +25405,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="308" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>17318</v>
       </c>
@@ -25482,7 +25467,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>17322</v>
       </c>
@@ -25544,7 +25529,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>17324</v>
       </c>
@@ -25594,7 +25579,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>17330</v>
       </c>
@@ -25656,7 +25641,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>17367</v>
       </c>
@@ -25718,7 +25703,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>17368</v>
       </c>
@@ -25780,7 +25765,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>17370</v>
       </c>
@@ -25842,7 +25827,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="315" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>17398</v>
       </c>
@@ -25904,7 +25889,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="316" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>17413</v>
       </c>
@@ -25966,7 +25951,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="317" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>17421</v>
       </c>
@@ -26028,7 +26013,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="318" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>17459</v>
       </c>
@@ -26090,7 +26075,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>17463</v>
       </c>
@@ -26152,7 +26137,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>17502</v>
       </c>
@@ -26214,7 +26199,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="321" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>17526</v>
       </c>
@@ -26276,7 +26261,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="322" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>17552</v>
       </c>
@@ -26338,7 +26323,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="323" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>17563</v>
       </c>
@@ -26400,7 +26385,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>17578</v>
       </c>
@@ -26462,7 +26447,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="325" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>17585</v>
       </c>
@@ -26527,7 +26512,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="326" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>17590</v>
       </c>
@@ -26589,7 +26574,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="327" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>17596</v>
       </c>
@@ -26703,7 +26688,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="329" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>17615</v>
       </c>
@@ -26765,7 +26750,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="330" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>17639</v>
       </c>
@@ -26827,7 +26812,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="331" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>17658</v>
       </c>
@@ -26889,7 +26874,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="332" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>17662</v>
       </c>
@@ -26951,7 +26936,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="333" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>17686</v>
       </c>
@@ -27013,7 +26998,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>17702</v>
       </c>
@@ -27075,7 +27060,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="335" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>18137</v>
       </c>
@@ -27137,7 +27122,7 @@
         <v>1543</v>
       </c>
     </row>
-    <row r="336" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>17706</v>
       </c>
@@ -27199,7 +27184,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="337" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>18855</v>
       </c>
@@ -27261,7 +27246,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="338" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>18866</v>
       </c>
@@ -27323,7 +27308,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="339" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>18867</v>
       </c>
@@ -27385,7 +27370,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="340" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>18870</v>
       </c>
@@ -27447,7 +27432,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="341" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>18878</v>
       </c>
@@ -27509,7 +27494,7 @@
         <v>1614</v>
       </c>
     </row>
-    <row r="342" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>18881</v>
       </c>
@@ -27559,7 +27544,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="343" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>18890</v>
       </c>
@@ -27621,7 +27606,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="344" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>18901</v>
       </c>
@@ -27683,7 +27668,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="345" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>18910</v>
       </c>
@@ -27745,7 +27730,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="346" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>18924</v>
       </c>
@@ -27807,7 +27792,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="347" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>17846</v>
       </c>
@@ -27857,7 +27842,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="348" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>17847</v>
       </c>
@@ -27919,7 +27904,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="349" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>17861</v>
       </c>
@@ -27981,7 +27966,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="350" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>17870</v>
       </c>
@@ -28043,7 +28028,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="351" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>17980</v>
       </c>
@@ -28105,7 +28090,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="352" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>17985</v>
       </c>
@@ -28167,7 +28152,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="353" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>18068</v>
       </c>
@@ -28229,7 +28214,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="354" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>18130</v>
       </c>
@@ -28291,7 +28276,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="355" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>18164</v>
       </c>
@@ -28353,7 +28338,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="356" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>18462</v>
       </c>
@@ -28415,7 +28400,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="357" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>18472</v>
       </c>
@@ -28477,7 +28462,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="358" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>18613</v>
       </c>
@@ -28539,7 +28524,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="359" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>18688</v>
       </c>
@@ -28601,7 +28586,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="360" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>18730</v>
       </c>
@@ -28663,7 +28648,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="361" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>18830</v>
       </c>
@@ -28725,7 +28710,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="362" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>19617</v>
       </c>
@@ -28787,7 +28772,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="363" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>19379</v>
       </c>
@@ -28849,7 +28834,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="364" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>19430</v>
       </c>
@@ -28911,7 +28896,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="365" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>19491</v>
       </c>
@@ -28973,7 +28958,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="366" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>19934</v>
       </c>
@@ -29035,7 +29020,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="367" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>19967</v>
       </c>
@@ -29097,7 +29082,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="368" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>19981</v>
       </c>
@@ -29159,7 +29144,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="369" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>20030</v>
       </c>
@@ -29221,7 +29206,7 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="370" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>20044</v>
       </c>
@@ -29283,7 +29268,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="371" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>20078</v>
       </c>
@@ -29345,7 +29330,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="372" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>20080</v>
       </c>
@@ -29407,7 +29392,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="373" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>20083</v>
       </c>
@@ -29469,7 +29454,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="374" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>20682</v>
       </c>
@@ -29531,7 +29516,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="375" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>20689</v>
       </c>
@@ -29581,7 +29566,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="376" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>20099</v>
       </c>
@@ -29643,7 +29628,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="377" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>19707</v>
       </c>
@@ -29705,7 +29690,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="378" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>20789</v>
       </c>
@@ -29767,7 +29752,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="379" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>20829</v>
       </c>
@@ -29829,7 +29814,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="380" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>20844</v>
       </c>
@@ -29891,7 +29876,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="381" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>20835</v>
       </c>
@@ -29953,7 +29938,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="382" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>20863</v>
       </c>
@@ -30003,7 +29988,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="383" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>20882</v>
       </c>
@@ -30065,7 +30050,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="384" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>20885</v>
       </c>
@@ -30127,7 +30112,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="385" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>21588</v>
       </c>
@@ -30177,7 +30162,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="386" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>23177</v>
       </c>
@@ -30239,7 +30224,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="387" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>23238</v>
       </c>
@@ -30301,7 +30286,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="388" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>23239</v>
       </c>
@@ -30363,7 +30348,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="389" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>23310</v>
       </c>
@@ -30413,7 +30398,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="390" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>22752</v>
       </c>
@@ -30475,7 +30460,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="391" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>22802</v>
       </c>
@@ -30489,7 +30474,7 @@
         <v>1600</v>
       </c>
       <c r="E391" s="8" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="F391" t="s">
         <v>64</v>
@@ -30537,7 +30522,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="392" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>22819</v>
       </c>
@@ -30551,7 +30536,7 @@
         <v>1591</v>
       </c>
       <c r="E392" s="8" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="F392" t="s">
         <v>51</v>
@@ -30599,7 +30584,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="393" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>22832</v>
       </c>
@@ -30613,7 +30598,7 @@
         <v>1597</v>
       </c>
       <c r="E393" s="8" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="F393" t="s">
         <v>19</v>
@@ -30661,7 +30646,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="394" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>22823</v>
       </c>
@@ -30675,7 +30660,7 @@
         <v>1594</v>
       </c>
       <c r="E394" s="8" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="F394" t="s">
         <v>64</v>
@@ -30723,7 +30708,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="395" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>22627</v>
       </c>
@@ -30785,7 +30770,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="396" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>24814</v>
       </c>
@@ -30847,7 +30832,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="397" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>27137</v>
       </c>
@@ -30909,7 +30894,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="398" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>27357</v>
       </c>
@@ -30971,7 +30956,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="399" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>26627</v>
       </c>
@@ -31006,7 +30991,7 @@
         <v>1675</v>
       </c>
       <c r="L399" t="s">
-        <v>108</v>
+        <v>1675</v>
       </c>
       <c r="M399" t="s">
         <v>1676</v>
@@ -31036,7 +31021,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="400" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>26739</v>
       </c>
@@ -31098,7 +31083,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="401" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>26784</v>
       </c>
@@ -31160,7 +31145,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="402" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>28939</v>
       </c>
@@ -31222,7 +31207,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="403" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>30490</v>
       </c>
@@ -31284,7 +31269,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="404" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>30509</v>
       </c>
@@ -31349,7 +31334,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="405" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>30524</v>
       </c>
@@ -31411,7 +31396,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="406" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>31322</v>
       </c>
@@ -31461,7 +31446,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="407" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>30329</v>
       </c>
@@ -31575,7 +31560,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="409" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>30047</v>
       </c>
@@ -31637,7 +31622,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="410" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>30057</v>
       </c>
@@ -31699,7 +31684,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="411" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>30061</v>
       </c>
@@ -31813,7 +31798,7 @@
         <v>1807</v>
       </c>
     </row>
-    <row r="413" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>30145</v>
       </c>
@@ -31875,7 +31860,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="414" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>30220</v>
       </c>
@@ -32001,7 +31986,13 @@
       <c r="E435"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T414" xr:uid="{19B4AC61-4D89-4886-A4F3-71B43E4AFDAA}"/>
+  <autoFilter ref="A1:T414" xr:uid="{19B4AC61-4D89-4886-A4F3-71B43E4AFDAA}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U414">
     <sortCondition ref="A1"/>
   </sortState>
@@ -32231,7 +32222,7 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32551,19 +32542,19 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>1987</v>
+      </c>
+      <c r="B7" t="s">
         <v>1988</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1988</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>1989</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1989</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1989</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>1990</v>
       </c>
       <c r="F7" t="s">
         <v>1689</v>
@@ -33049,19 +33040,19 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>1713</v>
       </c>
       <c r="C20" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1996</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>1997</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1997</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>1998</v>
       </c>
       <c r="F20" t="s">
         <v>1740</v>
@@ -33388,19 +33379,19 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>1713</v>
       </c>
       <c r="C29" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1994</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>1993</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1995</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>1994</v>
       </c>
       <c r="F29" t="s">
         <v>1717</v>
@@ -33485,7 +33476,7 @@
         <v>1720</v>
       </c>
       <c r="D31" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>1722</v>
@@ -33532,7 +33523,7 @@
         <v>1982</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="F32" t="s">
         <v>1717</v>
@@ -33573,7 +33564,7 @@
         <v>1724</v>
       </c>
       <c r="D33" t="s">
-        <v>1983</v>
+        <v>2014</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>1725</v>
@@ -33903,7 +33894,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="G6" s="14" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="H6" s="15">
         <f t="shared" ca="1" si="3"/>
@@ -34094,7 +34085,7 @@
       </c>
       <c r="E13" s="15">
         <f ca="1">SUM(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!L:L"),D13), COUNTIF(INDIRECT("'"&amp;$A$17:$A$17&amp;"'!L:L"),D13))</f>
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -34115,7 +34106,7 @@
       </c>
       <c r="E15" s="15">
         <f ca="1">SUM(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!L:L"),D15), COUNTIF(INDIRECT("'"&amp;$A$17:$A$17&amp;"'!L:L"),D15))</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -34362,7 +34353,7 @@
         <v>1676</v>
       </c>
       <c r="N4" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="O4" t="s">
         <v>1806</v>

</xml_diff>

<commit_message>
add recent new taxa
</commit_message>
<xml_diff>
--- a/resources/ABB_WorkingList_v1.0.xlsx
+++ b/resources/ABB_WorkingList_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72A54FA-7F90-43A6-8807-F3C1958D8975}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAD8181-C2C0-485E-BA13-E0C0F8DF8283}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{8E7CAC4A-2259-4D5B-9753-29EC3DCC188D}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB - Primary List" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7454" uniqueCount="2032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7468" uniqueCount="2036">
   <si>
     <t>Taxon Sort</t>
   </si>
@@ -6347,6 +6347,18 @@
   </si>
   <si>
     <t>901_Eastern Rosella_01.jpg</t>
+  </si>
+  <si>
+    <t>H12054</t>
+  </si>
+  <si>
+    <t>Trichoglossus haematodus x chlorolepidotus</t>
+  </si>
+  <si>
+    <t>Rainbow x Scaly-breasted Lorikeet</t>
+  </si>
+  <si>
+    <t>Rainbow x Scaly-breasted Lorikeet (hybrid)</t>
   </si>
 </sst>
 </file>
@@ -6925,9 +6937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787458D5-0D53-4EB5-974E-BD980B126E90}">
   <dimension ref="A1:U435"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H413" sqref="H413"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6996,7 +7008,7 @@
         <v>1921</v>
       </c>
       <c r="M1" s="6" t="str">
-        <f>"Draft: "&amp;SUM(COUNTIF(M2:M500,"Yes"),COUNTIF('ABB - Supplementary Lists'!M2:M500,"Yes"))</f>
+        <f>"Draft: "&amp;SUM(COUNTIF(M2:M500,"Yes"),COUNTIF('ABB - Supplementary Lists'!M2:M501,"Yes"))</f>
         <v>Draft: 56</v>
       </c>
       <c r="N1" s="6" t="s">
@@ -9613,7 +9625,7 @@
         <v>1671</v>
       </c>
       <c r="L43" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="M43" t="s">
         <v>1672</v>
@@ -32348,10 +32360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFAC224-3B06-46C1-8FBC-4E0275C3F461}">
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32359,7 +32371,7 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -33684,19 +33696,19 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>1972</v>
+        <v>2032</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>1709</v>
       </c>
       <c r="C33" t="s">
-        <v>1720</v>
+        <v>2035</v>
       </c>
       <c r="D33" t="s">
-        <v>2007</v>
+        <v>2034</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>1721</v>
+        <v>2033</v>
       </c>
       <c r="F33" t="s">
         <v>1713</v>
@@ -33726,8 +33738,52 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E35" s="10"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1720</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2007</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1713</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1714</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>1709</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>1709</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>1709</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1671</v>
+      </c>
+      <c r="L34" t="s">
+        <v>1671</v>
+      </c>
+      <c r="M34" t="s">
+        <v>1672</v>
+      </c>
+      <c r="N34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E36" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:T3" xr:uid="{C3BDEECB-DEA1-4819-8F62-78B8A91245CF}">
@@ -34138,7 +34194,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P9" s="16" t="s">
         <v>496</v>
@@ -34206,7 +34262,7 @@
       </c>
       <c r="B13" s="12">
         <f ca="1">SUM(B2:B10)</f>
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="14" t="s">
@@ -34214,7 +34270,7 @@
       </c>
       <c r="E13" s="15">
         <f ca="1">SUM(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!L:L"),D13), COUNTIF(INDIRECT("'"&amp;$A$17:$A$17&amp;"'!L:L"),D13))</f>
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -34223,7 +34279,7 @@
       </c>
       <c r="E14" s="16">
         <f ca="1">SUM(COUNTIF(INDIRECT("'"&amp;$A$16:$A$16&amp;"'!L:L"),D14), COUNTIF(INDIRECT("'"&amp;$A$17:$A$17&amp;"'!L:L"),D14))</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -34252,7 +34308,7 @@
       </c>
       <c r="E17" s="12">
         <f ca="1">SUM(E13:E15)</f>
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>